<commit_message>
sync primary outputJob files
</commit_message>
<xml_diff>
--- a/Bill of Materials-Michel.xlsx
+++ b/Bill of Materials-Michel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32925" windowHeight="15825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19980"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Michel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="511">
   <si>
     <t>Designator</t>
   </si>
@@ -54,7 +54,7 @@
     <t>DataSheet</t>
   </si>
   <si>
-    <t>C1, C3, C4, C5, C6, C7, C8, C9, C16_Audio Input L, C16_Audio Input R, C16_Audio Repeat L, C16_Audio Repeat R, C18_Audio Input L, C18_Audio Input R, C18_Audio Repeat L, C18_Audio Repeat R, C22_Audio Output1, C22_Audio Output2, C22_Audio Output3, C23_Audio Output1, C23_Audio Output2, C23_Audio Output3, C24_Audio Output1, C24_Audio Output2, C24_Audio Output3, C25_Audio Output1, C25_Audio Output2, C25_Audio Output3, C26_Audio Output1, C26_Audio Output2, C26_Audio Output3, C27_Audio Output1, C27_Audio Output2, C27_Audio Output3, C166, C167, C168, C169</t>
+    <t>C1, C3, C4, C5, C6, C7, C12, C13, C17_Audio Input L, C17_Audio Input R, C17_Audio Repeat L, C17_Audio Repeat R, C18_Audio Input L, C18_Audio Input R, C18_Audio Repeat L, C18_Audio Repeat R, C22_Audio Output1, C22_Audio Output2, C22_Audio Output3, C23_Audio Output1, C23_Audio Output2, C23_Audio Output3, C24_Audio Output1, C24_Audio Output2, C24_Audio Output3, C25_Audio Output1, C25_Audio Output2, C25_Audio Output3, C26_Audio Output1, C26_Audio Output2, C26_Audio Output3, C27_Audio Output1, C27_Audio Output2, C27_Audio Output3, C166, C167, C168, C169</t>
   </si>
   <si>
     <t>1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 0.01uF, 0.01uF, 0.01uF, 0.01uF, 2200pF, 2200pF, 2200pF, 2200pF, 330pF, 330pF, 330pF, 1500pF, 1500pF, 1500pF, 330pF, 330pF, 330pF, 330pF, 330pF, 330pF, 1500pF, 1500pF, 1500pF, 330pF, 330pF, 330pF, 0.1uF, 0.1uF, 0.1uF, 0.1uF</t>
@@ -84,7 +84,7 @@
     <t>http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048127.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2165971.pdf, http://www.farnell.com/datasheets/2165971.pdf, http://www.farnell.com/datasheets/2165971.pdf, http://www.farnell.com/datasheets/2165971.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165940.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2165943.pdf, http://www.farnell.com/datasheets/2048172.pdf, http://www.farnell.com/datasheets/2048172.pdf, http://www.farnell.com/datasheets/2048172.pdf, http://www.farnell.com/datasheets/2048172.pdf</t>
   </si>
   <si>
-    <t>C2, C10, C11, C12, C13, C14, C17_Audio Input L, C17_Audio Input R, C17_Audio Repeat L, C17_Audio Repeat R, C30, C33, C44, C49, C58, C63, C65_MS - LR Converter1, C65_MS - LR Converter2, C66_MS - LR Converter1, C66_MS - LR Converter2, C114_Mode Select 1A, C114_Mode Select 1B, C114_Mode Select 2A, C114_Mode Select 2B</t>
+    <t>C2, C8, C9, C10, C11, C14, C16_Audio Input L, C16_Audio Input R, C16_Audio Repeat L, C16_Audio Repeat R, C30, C33, C44, C49, C58, C63, C114_Mode Select 1A, C114_Mode Select 1B, C114_Mode Select 2A, C114_Mode Select 2B, C?, C?, C?, C?, C?</t>
   </si>
   <si>
     <t>10uF</t>
@@ -105,7 +105,7 @@
     <t>http://www.farnell.com/datasheets/2079165.pdf</t>
   </si>
   <si>
-    <t>C15_Audio Input L, C15_Audio Input R, C15_Audio Repeat L, C15_Audio Repeat R, C31, C34, C36, C41, C46, C60, C72, C74, C127, C130, C131, C134</t>
+    <t>C15_Audio Input L, C15_Audio Input R, C15_Audio Repeat L, C15_Audio Repeat R, C31, C34, C36, C41, C46, C60, C72, C74, C127, C130, C131, C134, C?_MS - LR Converter1, C?_MS - LR Converter1, C?_MS - LR Converter2, C?_MS - LR Converter2</t>
   </si>
   <si>
     <t>22uF</t>
@@ -117,10 +117,10 @@
     <t>2666490</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf</t>
-  </si>
-  <si>
-    <t>C19_Audio Input L, C19_Audio Input R, C19_Audio Repeat L, C19_Audio Repeat R, C20_Audio Input L, C20_Audio Input R, C20_Audio Repeat L, C20_Audio Repeat R, C21_Audio Input L, C21_Audio Input R, C21_Audio Repeat L, C21_Audio Repeat R, C28_Audio Output1, C28_Audio Output2, C28_Audio Output3, C29_Audio Output1, C29_Audio Output2, C29_Audio Output3, C51, C52, C53, C54, C55, C67_MS - LR Converter1, C67_MS - LR Converter2, C68_MS - LR Converter1, C68_MS - LR Converter2, C69_MS - LR Converter1, C69_MS - LR Converter2, C70_MS - LR Converter1, C70_MS - LR Converter2, C71_MS - LR Converter1, C71_MS - LR Converter2, C76, C77, C78, C79, C86, C87, C88, C95, C96, C103, C104, C105, C112, C113, C115_Mode Select 1A, C115_Mode Select 1B, C115_Mode Select 2A, C115_Mode Select 2B, C116, C117, C118, C119, C120, C121, C122, C123, C124, C125, C126, C135, C136, C137, C138, C139, C243, C263</t>
+    <t>http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf</t>
+  </si>
+  <si>
+    <t>C19_Audio Input L, C19_Audio Input R, C19_Audio Repeat L, C19_Audio Repeat R, C20_Audio Input L, C20_Audio Input R, C20_Audio Repeat L, C20_Audio Repeat R, C21_Audio Input L, C21_Audio Input R, C21_Audio Repeat L, C21_Audio Repeat R, C28_Audio Output1, C28_Audio Output2, C28_Audio Output3, C29_Audio Output1, C29_Audio Output2, C29_Audio Output3, C51, C52, C53, C54, C55, C67_MS - LR Converter1, C67_MS - LR Converter2, C68_MS - LR Converter1, C68_MS - LR Converter2, C69_MS - LR Converter1, C69_MS - LR Converter2, C70_MS - LR Converter1, C70_MS - LR Converter2, C71_MS - LR Converter1, C71_MS - LR Converter2, C76, C77, C78, C79, C86, C87, C88, C95, C96, C103, C104, C105, C112, C113, C115_Mode Select 1A, C115_Mode Select 1B, C115_Mode Select 2A, C115_Mode Select 2B, C116, C117, C118, C119, C120, C121, C122, C123, C124, C125, C126, C135, C136, C137, C139, C243, C263, C?, C?</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -270,67 +270,100 @@
     <t>http://www.farnell.com/datasheets/2165937.pdf</t>
   </si>
   <si>
-    <t>C140, C143, C146, C149</t>
-  </si>
-  <si>
-    <t>24pF</t>
+    <t>C138, C171, C172, C173, C174, C242, C244, C245, C246, C247, C248, C249, C250, C251, C252, C253, C254, C255, C256, C257, C258, C259, C260, C261, C262, C264, C266, C267, C268, C269, C270, C271, C272, C273, C274, C275, C276, C277, C278, C279, C280</t>
+  </si>
+  <si>
+    <t>10uF, 1nF, 1nF, 1nF, 1nF, 22uF, 4.7uF, 22uF, 10uF, 100nF, 22uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 2.2uF, 10uF, 2.2uF, 4.7uF, 4.7uF, 10uF, 10uF, 0.1uF, 10uF, 0.1uF, 0.1uF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF</t>
   </si>
   <si>
     <t>Capacitor</t>
   </si>
   <si>
-    <t>GRM1555C1H240JA01D</t>
-  </si>
-  <si>
-    <t>2218850</t>
+    <t>GRM188R60J106ME47J, GRM1555C1H102GA01D, GRM1555C1H102GA01D, GRM1555C1H102GA01D, GRM1555C1H102GA01D, ZRB18AR60J226ME01L, GRM188R60J475KE19D, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188F51E104ZA01D, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J475KE19D, GRM188R60J475KE19D, GRM188R60J106ME47J, GRM188R60J106ME47J, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T</t>
+  </si>
+  <si>
+    <t>MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>2611921, 2470453, 2470453, 2470453, 2470453, 2666613, 2666491, 2666490, 2611921, 1828902, 2666490, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2672153, 2611921, 2672153, 2666491, 2666491, 2611921, 2611921, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069, 2113069</t>
+  </si>
+  <si>
+    <t>RAD-0.3</t>
+  </si>
+  <si>
+    <t>0603 [1608 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric]</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2163235.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf</t>
+  </si>
+  <si>
+    <t>C141, C143, C144, C147, C148, C150, C151, C152, C153, C154, C155, C156, C157, C158, C159, C160, C161, C162, C164, C165, C176, C177, C178, C180, C181, C182, C183, C184, C185, C186, C187, C188, C189, C190, C191, C192, C193, C194, C195, C196, C197, C198, C199, C200, C201, C202, C203, C204, C205, C206, C207, C208, C209, C210, C215, C216, C217, C218, C219, C220, C221, C222, C224, C225, C226, C227, C228, C229, C230, C231, C232, C236, C237, C238, C239, C240</t>
+  </si>
+  <si>
+    <t>GRM155R61A104JA01D</t>
+  </si>
+  <si>
+    <t>2470461</t>
+  </si>
+  <si>
+    <t>0402 [1005 Metric]</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2048172.pdf</t>
+  </si>
+  <si>
+    <t>C142, C145</t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>GRM0335C1E180JA01D</t>
+  </si>
+  <si>
+    <t>2434635</t>
   </si>
   <si>
     <t>0402</t>
   </si>
   <si>
-    <t>0402 [1005 Metric]</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2048357.pdf</t>
-  </si>
-  <si>
-    <t>C141, C171, C172, C173, C174, C242, C244, C245, C246, C247, C248, C249, C250, C251, C252, C253, C254, C255, C256, C257, C258, C259, C260, C261, C262, C264, C265, C?, C?, C?</t>
-  </si>
-  <si>
-    <t>33pF, 1nF, 1nF, 1nF, 1nF, 22uF, 4.7uF, 22uF, 10uF, 100nF, 22uF, 22uF, 10uF, 22uF, 10uF, 22uF, 10uF, 10uF, 2.2uF, 10uF, 2.2uF, 4.7uF, 4.7uF, 10uF, 10uF, XXXuF, 0.1uF, 10uF, 0.1uF, 0.1uF</t>
-  </si>
-  <si>
-    <t>GRT1885C1H330JA02D, GRM1555C1H102GA01D, GRM1555C1H102GA01D, GRM1555C1H102GA01D, GRM1555C1H102GA01D, ZRB18AR60J226ME01L, GRM188R60J475KE19D, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188F51E104ZA01D, GRM188R60J226MEA0D, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J475KE19D, GRM188R60J475KE19D, GRM188R60J106ME47J, GRM188R60J106ME47J, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T, JMK212BJ226KG-T</t>
-  </si>
-  <si>
-    <t>MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, MURATA, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN, TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>2672141, 2470453, 2470453, 2470453, 2470453, 2666613, 2666491, 2666490, 2611921, 1828902, 2666490, 2666490, 2611921, 2666490, 2611921, 2666490, 2611921, 2611921, 2672153, 2611921, 2672153, 2666491, 2666491, 2611921, 2611921, 2113069, 2113069, 2113069, 2113069, 2113069</t>
-  </si>
-  <si>
-    <t>RAD-0.3</t>
-  </si>
-  <si>
-    <t>0603 [1608 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0402 [1005 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric]</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2165942.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2048131.pdf, http://www.farnell.com/datasheets/2163235.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf, http://www.farnell.com/datasheets/1910934.pdf</t>
-  </si>
-  <si>
-    <t>C142, C144, C145, C147, C148, C150, C151, C152, C153, C154, C155, C156, C157, C158, C159, C160, C161, C162, C163, C164, C165, C170, C175, C177, C178, C180, C181, C182, C183, C184, C185, C186, C187, C188, C189, C190, C191, C192, C193, C194, C195, C196, C197, C198, C199, C200, C201, C202, C203, C204, C205, C206, C207, C208, C209, C210, C215, C216, C217, C218, C219, C220, C221, C223, C224, C225, C226, C227, C228, C229, C230, C231, C232, C236, C237, C238, C239, C240</t>
-  </si>
-  <si>
-    <t>GRM155R61A104JA01D</t>
-  </si>
-  <si>
-    <t>2470461</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2048172.pdf</t>
-  </si>
-  <si>
-    <t>C176, C233, C235</t>
+    <t>0201 [0603 Metric]</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2048029.pdf</t>
+  </si>
+  <si>
+    <t>C146, C149</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>GRM0335C1E120JA01D</t>
+  </si>
+  <si>
+    <t>2434633</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2047992.pdf</t>
+  </si>
+  <si>
+    <t>C163, C170</t>
+  </si>
+  <si>
+    <t>C0201C104K9PACTU</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>1907036</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2580263.pdf</t>
+  </si>
+  <si>
+    <t>C175, C233, C235</t>
   </si>
   <si>
     <t>10nf, 100pF, 100pF</t>
@@ -345,7 +378,7 @@
     <t>http://www.farnell.com/datasheets/2048220.pdf</t>
   </si>
   <si>
-    <t>C179, C211, C222, C241</t>
+    <t>C179, C211, C223, C241, C?</t>
   </si>
   <si>
     <t>GRM155R61A224KE19D</t>
@@ -357,7 +390,7 @@
     <t>http://www.farnell.com/datasheets/2048289.pdf</t>
   </si>
   <si>
-    <t>C212, C213, C214, C234</t>
+    <t>C212, C213, C214, C234, C?</t>
   </si>
   <si>
     <t>GRT155C81A105KE01D</t>
@@ -420,25 +453,28 @@
     <t>http://www.ti.com/lit/ds/symlink/lm4041-n.pdf</t>
   </si>
   <si>
-    <t>D19, D20, D21, D22, D23, D24, D25, D26, D27, D28, D29, D30, D31, D32, D33, D34, D35, D36, D37, D38, D39, D40, D41, D42, D43, D44, D45, D46, D47, D48, D49, D50, D51, D52, D53, D54, D55, D56, D57, D58, D59, D60, D61, D62, D63, D64, D65, D66, D67, D68, D69, D70, D71, D72, D73, D74, D75, D76, D77, D78, D79, D80, D81, D82, D83</t>
+    <t>D19, D20, D21, D22, D23, D24, D25, D26, D27, D28, D29, D30, D31, D32, D33, D34, D35, D36, D37, D38, D39, D40, D41, D42, D43, D44, D45, D46, D47, D48, D49, D50, D51, D52, D53, D54, D55, D56, D57, D58, D59, D60, D61, D62, D63, D64, D65, D66, D67</t>
   </si>
   <si>
     <t>Typical INFRARED GaAs LED</t>
   </si>
   <si>
-    <t>LNJ037X8ARA</t>
-  </si>
-  <si>
-    <t>1908051</t>
+    <t>VLMW41S1T1-8K8L-08, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA, LNJ037X8ARA</t>
+  </si>
+  <si>
+    <t>VISHAY, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS, PANASONIC ELECTRONIC COMPONENTS</t>
+  </si>
+  <si>
+    <t>2251500, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051, 1908051</t>
   </si>
   <si>
     <t>LED-0</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/2085723.pdf</t>
-  </si>
-  <si>
-    <t>G1</t>
+    <t>http://www.farnell.com/datasheets/2050239.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf, http://www.farnell.com/datasheets/2085723.pdf</t>
+  </si>
+  <si>
+    <t>G?</t>
   </si>
   <si>
     <t>Ground Ultime</t>
@@ -462,25 +498,19 @@
     <t>1854512</t>
   </si>
   <si>
+    <t>CLIFF ELECTRONIC COMPONENTS_FC681465P</t>
+  </si>
+  <si>
     <t>http://www.farnell.com/datasheets/1855458.pdf</t>
   </si>
   <si>
-    <t>J2, J3</t>
+    <t>J2, J3, J7</t>
   </si>
   <si>
     <t>Dual Jack stereo bypassed</t>
   </si>
   <si>
-    <t>ACJS-MHDC</t>
-  </si>
-  <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
-    <t>2771861</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/cad/2158945.pdf</t>
+    <t>JACK/6-V4A</t>
   </si>
   <si>
     <t>J4</t>
@@ -489,31 +519,43 @@
     <t>Connecteurs carte à carte</t>
   </si>
   <si>
-    <t>2211S-05G</t>
-  </si>
-  <si>
-    <t>multicomp</t>
-  </si>
-  <si>
-    <t>1593414</t>
+    <t>TSM-103-01-T-DV</t>
+  </si>
+  <si>
+    <t>SAMTEC</t>
+  </si>
+  <si>
+    <t>2505049</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2186767.pdf</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>2 Pads</t>
+  </si>
+  <si>
+    <t>2211S-02G</t>
+  </si>
+  <si>
+    <t>1593411</t>
+  </si>
+  <si>
+    <t>HDR1X2</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/1518407.pdf</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>2 Pads</t>
-  </si>
-  <si>
-    <t>2211S-02G</t>
-  </si>
-  <si>
-    <t>1593411</t>
-  </si>
-  <si>
-    <t>HDR1X2</t>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>Pad traversant</t>
+  </si>
+  <si>
+    <t>Pad</t>
   </si>
   <si>
     <t>L1, L2, L3</t>
@@ -567,6 +609,21 @@
     <t>http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/datasheets/321059.pdf</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Protoboard Olimex</t>
+  </si>
+  <si>
+    <t>AM3352-SOM-EVB</t>
+  </si>
+  <si>
+    <t>Olimex</t>
+  </si>
+  <si>
+    <t>https://www.olimex.com/Products/SOM/AM335X/AM3352-SOM/resources/AM3352-SOM-UM.pdf</t>
+  </si>
+  <si>
     <t>P2, P3</t>
   </si>
   <si>
@@ -624,58 +681,43 @@
     <t>http://www.farnell.com/datasheets/1912447.pdf</t>
   </si>
   <si>
-    <t>P?</t>
-  </si>
-  <si>
-    <t>Protoboard Olimex</t>
-  </si>
-  <si>
-    <t>AM3352-SOM-EVB</t>
-  </si>
-  <si>
-    <t>Olimex</t>
-  </si>
-  <si>
-    <t>https://www.olimex.com/Products/SOM/AM335X/AM3352-SOM/resources/AM3352-SOM-UM.pdf</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
-    <t>24MHz</t>
+    <t>ABMM2-24.000MHZ-E2-T</t>
+  </si>
+  <si>
+    <t>ABRACON</t>
+  </si>
+  <si>
+    <t>2467855</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1750519.pdf</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>32,768KHz</t>
   </si>
   <si>
     <t>Crystal Oscillator</t>
   </si>
   <si>
-    <t>QX233A24.00000B15M</t>
-  </si>
-  <si>
-    <t>QANTEK TECHNOLOGY CORPORATION</t>
-  </si>
-  <si>
-    <t>2508810</t>
+    <t>LFXTAL003000</t>
+  </si>
+  <si>
+    <t>IQD FREQUENCY PRODUCTS</t>
+  </si>
+  <si>
+    <t>9713220</t>
   </si>
   <si>
     <t>R38</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/1998823.pdf</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>ASFLK-32.768KHZ-LJT</t>
-  </si>
-  <si>
-    <t>ABRACON</t>
-  </si>
-  <si>
-    <t>2101317</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1738890.pdf</t>
+    <t>http://www.farnell.com/datasheets/2175893.pdf</t>
   </si>
   <si>
     <t>Q3</t>
@@ -720,7 +762,7 @@
     <t>http://www.farnell.com/datasheets/2237089.pdf</t>
   </si>
   <si>
-    <t>Q?</t>
+    <t>Q5</t>
   </si>
   <si>
     <t>8MHz</t>
@@ -738,31 +780,31 @@
     <t>http://www.farnell.com/datasheets/1506176.pdf</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13_Audio Input L, R13_Audio Input R, R13_Audio Repeat L, R13_Audio Repeat R, R14_Audio Input L, R14_Audio Input R, R14_Audio Repeat L, R14_Audio Repeat R, R15_Audio Input L, R15_Audio Input R, R15_Audio Repeat L, R15_Audio Repeat R, R16_Audio Input L, R16_Audio Input R, R16_Audio Repeat L, R16_Audio Repeat R, R17_Audio Input L, R17_Audio Input R, R17_Audio Repeat L, R17_Audio Repeat R, R18_Audio Input L, R18_Audio Input R, R18_Audio Repeat L, R18_Audio Repeat R, R19_Audio Output1, R19_Audio Output2, R19_Audio Output3, R20_Audio Output1, R20_Audio Output2, R20_Audio Output3, R21_Audio Output1, R21_Audio Output2, R21_Audio Output3, R22_Audio Output1, R22_Audio Output2, R22_Audio Output3, R23_Audio Output1, R23_Audio Output2, R23_Audio Output3, R24_Audio Output1, R24_Audio Output2, R24_Audio Output3, R25_Audio Output1, R25_Audio Output2, R25_Audio Output3, R26_Audio Output1, R26_Audio Output2, R26_Audio Output3, R27_Audio Output1, R27_Audio Output2, R27_Audio Output3, R28_Audio Output1, R28_Audio Output2, R28_Audio Output3, R29_Audio Output1, R29_Audio Output2, R29_Audio Output3, R30_Audio Output1, R30_Audio Output2, R30_Audio Output3, R31_Audio Output1, R31_Audio Output2, R31_Audio Output3, R32_Audio Output1, R32_Audio Output2, R32_Audio Output3, R270, R271, R272, R273, R274, R275, R276, R277</t>
-  </si>
-  <si>
-    <t>0, 0, 0, 0, 0, 0, 0, 0, 10k, 10k, 10k, 10k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 1.5k, 1.5k, 1.5k, 1.5k, 3k, 3k, 3k, 3k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 10k, 20k, 10k, 20k, 10k, 20k, 10k, 20k</t>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13_Audio Input L, R13_Audio Input R, R13_Audio Repeat L, R13_Audio Repeat R, R14_Audio Input L, R14_Audio Input R, R14_Audio Repeat L, R14_Audio Repeat R, R15_Audio Input L, R15_Audio Input R, R15_Audio Repeat L, R15_Audio Repeat R, R16_Audio Input L, R16_Audio Input R, R16_Audio Repeat L, R16_Audio Repeat R, R17_Audio Input L, R17_Audio Input R, R17_Audio Repeat L, R17_Audio Repeat R, R18_Audio Input L, R18_Audio Input R, R18_Audio Repeat L, R18_Audio Repeat R, R19_Audio Output1, R19_Audio Output2, R19_Audio Output3, R20_Audio Output1, R20_Audio Output2, R20_Audio Output3, R21_Audio Output1, R21_Audio Output2, R21_Audio Output3, R22_Audio Output1, R22_Audio Output2, R22_Audio Output3, R23_Audio Output1, R23_Audio Output2, R23_Audio Output3, R24_Audio Output1, R24_Audio Output2, R24_Audio Output3, R25_Audio Output1, R25_Audio Output2, R25_Audio Output3, R26_Audio Output1, R26_Audio Output2, R26_Audio Output3, R27_Audio Output1, R27_Audio Output2, R27_Audio Output3, R28_Audio Output1, R28_Audio Output2, R28_Audio Output3, R29_Audio Output1, R29_Audio Output2, R29_Audio Output3, R30_Audio Output1, R30_Audio Output2, R30_Audio Output3, R31_Audio Output1, R31_Audio Output2, R31_Audio Output3, R32_Audio Output1, R32_Audio Output2, R32_Audio Output3, R271, R272, R273, R274, R275, R276, R277</t>
+  </si>
+  <si>
+    <t>0, 0, 0, 0, 0, 0, 0, 0, 10k, 10k, 0, 10k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 1.5k, 1.5k, 1.5k, 1.5k, 3k, 3k, 3k, 3k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 20k, 10k, 20k, 10k, 20k, 10k, 20k</t>
   </si>
   <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, TDK, TDK, TDK, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TDK, TDK, TDK, TE CONNECTIVITY, TDK, TE CONNECTIVITY, TDK, TE CONNECTIVITY, TDK, TE CONNECTIVITY, TDK</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2483933, 2483933, 2483933, 2483933, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2613050, 2613050, 2613050, 2613050, 2331191, 2331191, 2331191, 2331191, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029</t>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, [NoParam], CPF-A-0603B4K7E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], TE CONNECTIVITY, TE CONNECTIVITY, [NoParam], TE CONNECTIVITY, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, TDK, TDK, TDK, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, KEMET, TDK, TDK, TDK, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TDK, TDK, TDK, TDK, TE CONNECTIVITY, TDK, TE CONNECTIVITY, TDK, TE CONNECTIVITY, TDK</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2483933, 2483933, [NoParam], 2483933, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2613050, 2613050, 2613050, 2613050, 2331191, 2331191, 2331191, 2331191, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2331029, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029</t>
   </si>
   <si>
     <t>J1-0603</t>
   </si>
   <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric]</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf</t>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 0603 [1608 Metric], 0603 [1608 Metric], [NoParam], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric], 0603 [1608 Metric], 0805 [2012 Metric]</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf</t>
   </si>
   <si>
     <t>R33, R34, R35, R36, R49, R50, R51, R80_MS - LR Converter1, R80_MS - LR Converter2, R81_MS - LR Converter1, R81_MS - LR Converter2, R82, R86, R110, R111, R112, R153, R154, R155, R177_Mode Select 1A, R177_Mode Select 1B, R177_Mode Select 2A, R177_Mode Select 2B, R178_Mode Select 1A, R178_Mode Select 1B, R178_Mode Select 2A, R178_Mode Select 2B, R179_Mode Select 1A, R179_Mode Select 1B, R179_Mode Select 2A, R179_Mode Select 2B, R180, R181, R191, R192, R193, R208, R209, R210, R211, R212, R213</t>
@@ -789,7 +831,7 @@
     <t>http://www.farnell.com/datasheets/1935020.pdf</t>
   </si>
   <si>
-    <t>R40, R42, R47, R55, R57, R62, R83, R87, R90, R91, R92, R107, R109, R113, R114, R115, R130, R132, R133, R134, R135, R150, R152, R156, R157, R158, R173, R175, R184, R185, R190, R196, R197, R202</t>
+    <t>R40, R42, R47, R55, R57, R62, R83, R87, R90, R91, R92, R107, R109, R113, R114, R115, R130, R132, R133, R134, R135, R150, R152, R156, R157, R158, R173, R175, R184, R185, R190, R196, R197, R202, R?_MS - LR Converter1, R?_MS - LR Converter1, R?_MS - LR Converter2, R?_MS - LR Converter2</t>
   </si>
   <si>
     <t>100k</t>
@@ -798,16 +840,13 @@
     <t>RN73C1J100KBTDF</t>
   </si>
   <si>
-    <t>KEMET</t>
-  </si>
-  <si>
     <t>2687850</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2189072.pdf</t>
   </si>
   <si>
-    <t>R44, R203, R206, R207</t>
+    <t>R44, R203, R206, R207, R?</t>
   </si>
   <si>
     <t>220k</t>
@@ -819,10 +858,61 @@
     <t>2483903</t>
   </si>
   <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>R70_MS - LR Converter1, R70_MS - LR Converter2, R79_MS - LR Converter1, R79_MS - LR Converter2, R176_Mode Select 1A, R176_Mode Select 1B, R176_Mode Select 2A, R176_Mode Select 2B</t>
+    <t>R85, R89</t>
+  </si>
+  <si>
+    <t>13k</t>
+  </si>
+  <si>
+    <t>CPF0603B13KE1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>2330920</t>
+  </si>
+  <si>
+    <t>0805 [2012 Metric]</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2104089.pdf</t>
+  </si>
+  <si>
+    <t>R93, R94, R95, R96, R97, R98, R101, R106, R116, R117, R118, R119, R120, R121, R124, R129, R136, R137, R138, R139, R140, R141, R144, R149, R159, R160, R161, R162, R163, R164, R167, R172, R?</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B33KE1</t>
+  </si>
+  <si>
+    <t>2483920</t>
+  </si>
+  <si>
+    <t>R102, R103, R125, R126, R145, R146, R168, R169</t>
+  </si>
+  <si>
+    <t>51k</t>
+  </si>
+  <si>
+    <t>CPF0603B51KE1</t>
+  </si>
+  <si>
+    <t>2331265</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2043335.pdf</t>
+  </si>
+  <si>
+    <t>R104, R105, R127, R128, R147, R148, R170, R171, R189, R201</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>R176_Mode Select 1A, R176_Mode Select 1B, R176_Mode Select 2A, R176_Mode Select 2B</t>
   </si>
   <si>
     <t>470k</t>
@@ -834,61 +924,7 @@
     <t>2331232</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/2043335.pdf</t>
-  </si>
-  <si>
-    <t>R85, R89</t>
-  </si>
-  <si>
-    <t>13k</t>
-  </si>
-  <si>
-    <t>CPF0603B13KE1</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>2330920</t>
-  </si>
-  <si>
-    <t>0805 [2012 Metric]</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2104089.pdf</t>
-  </si>
-  <si>
-    <t>R93, R94, R95, R96, R97, R98, R99, R100, R101, R106, R116, R117, R118, R119, R120, R121, R122, R123, R124, R129, R136, R137, R138, R139, R140, R141, R142, R143, R144, R149, R159, R160, R161, R162, R163, R164, R165, R166, R167, R172</t>
-  </si>
-  <si>
-    <t>33k</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B33KE1</t>
-  </si>
-  <si>
-    <t>2483920</t>
-  </si>
-  <si>
-    <t>R102, R103, R125, R126, R145, R146, R168, R169</t>
-  </si>
-  <si>
-    <t>51k</t>
-  </si>
-  <si>
-    <t>CPF0603B51KE1</t>
-  </si>
-  <si>
-    <t>2331265</t>
-  </si>
-  <si>
-    <t>R104, R105, R127, R128, R147, R148, R170, R171, R189, R201</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>R182, R194, R205</t>
+    <t>R182, R194, R205, R?, R?, R?, R?, R?, R?, R?, R?</t>
   </si>
   <si>
     <t>1k</t>
@@ -939,33 +975,42 @@
     <t>R221</t>
   </si>
   <si>
-    <t>R223, R224, R225, R226, R227, R228, R229, R230, R231, R232, R233, R234, R235, R236, R237, R238, R239, R240, R241, R242, R243, R244, R245, R246, R247, R248, R249, R250, R251, R252, R253, R254, R255, R256, R257, R258, R259, R260, R261, R262, R263, R264, R265, R266, R267, R268, R269, R284, R285</t>
-  </si>
-  <si>
-    <t>1.2k, 0, DNI, 10k, DNI, DNI, 100K, DNI, DNI, DNI, DNI, DNI, DNI, 100K, DNI, DNI, DNI, DNI, 100K, DNI, 100K, 100K, DNI, 100K, 100K, 100K, 100K, 100K, 100K, DNI, 100K, 100K, 100K, 100K, DNI, 100K, 10k, 10k, 10k, 10k, 10k, 0, 0, 10k, 100k, 0, 0, 10k, XXX</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B1K2E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, RN73C1J100KBTDF, [NoParam], [NoParam], CPF-A-0603B4K7E1, [NoParam]</t>
-  </si>
-  <si>
-    <t>KEMET, [NoParam], [NoParam], TE CONNECTIVITY, [NoParam], [NoParam], KEMET, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], KEMET, [NoParam], [NoParam], [NoParam], [NoParam], KEMET, [NoParam], KEMET, KEMET, [NoParam], KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, [NoParam], KEMET, KEMET, KEMET, KEMET, [NoParam], KEMET, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, [NoParam], [NoParam], TE CONNECTIVITY, KEMET, [NoParam], [NoParam], TE CONNECTIVITY, [NoParam]</t>
-  </si>
-  <si>
-    <t>2483896, [NoParam], [NoParam], 2483933, [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2483933, 2483933, 2483933, 2483933, 2483933, [NoParam], [NoParam], 2483933, 2687850, [NoParam], [NoParam], 2483933, [NoParam]</t>
+    <t>R223, R224, R225, R226, R227, R228, R229, R230, R231, R232, R233, R234, R235, R236, R237, R238, R239, R240, R241, R242, R243, R244, R245, R246, R247, R248, R249, R250, R251, R252, R253, R254, R255, R256, R257, R258, R259, R260, R261, R262, R263, R264, R265, R266, R266, R267, R267, R268, R269, R270, R278, R286, R287, R288, R289, R290, R291, R292, R293, R294, R295, R296, R297, R298, R299, R300, R301, R302, R303, R304, R305, R306, R307, R308, R309</t>
+  </si>
+  <si>
+    <t>1.2k, 0, DNI, 10k, DNI, DNI, 100K, DNI, DNI, DNI, DNI, DNI, DNI, 100K, DNI, DNI, DNI, DNI, 100K, DNI, 100K, 100K, DNI, 100K, 100K, 100K, 100K, 100K, 100K, DNI, 100K, 100K, 100K, 100K, DNI, 100K, 10k, 10k, 10k, 10k, 10k, 0, 0, 10k, 10k, 100k, 100k, 0, 0, 10k, 10k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B1K2E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>KEMET, [NoParam], [NoParam], TE CONNECTIVITY, [NoParam], [NoParam], KEMET, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], KEMET, [NoParam], [NoParam], [NoParam], [NoParam], KEMET, [NoParam], KEMET, KEMET, [NoParam], KEMET, KEMET, KEMET, KEMET, KEMET, KEMET, [NoParam], KEMET, KEMET, KEMET, KEMET, [NoParam], KEMET, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, TE CONNECTIVITY, [NoParam], [NoParam], TE CONNECTIVITY, TE CONNECTIVITY, KEMET, KEMET, [NoParam], [NoParam], TE CONNECTIVITY, TE CONNECTIVITY, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>2483896, [NoParam], [NoParam], 2483933, [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2483933, 2483933, 2483933, 2483933, 2483933, [NoParam], [NoParam], 2483933, 2483933, 2687850, 2687850, [NoParam], [NoParam], 2483933, 2483933, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam]</t>
   </si>
   <si>
     <t>AXIAL-0.3</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, [NoParam]</t>
-  </si>
-  <si>
-    <t>R278, R279, R280, R281, R282, R283</t>
+    <t>http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>R279, R280, R281, R282, R283, R284</t>
   </si>
   <si>
     <t>Potentiometer</t>
   </si>
   <si>
+    <t>RK09K1130C79, RK09K1130C79, P160KMP-0QC20B10K, P160KMP-0QC20B10K, P160KMP-0QC20B10K, P160KMP-0QC20B10K</t>
+  </si>
+  <si>
+    <t>ALPS, ALPS, Bi Technology, Bi Technology, Bi Technology, Bi Technology</t>
+  </si>
+  <si>
+    <t>1191741, 1191741, 1760793, 1760793, 1760793, 1760793</t>
+  </si>
+  <si>
     <t>VR5</t>
   </si>
   <si>
@@ -996,6 +1041,9 @@
     <t>PCM3168APAP</t>
   </si>
   <si>
+    <t>TEXAS INSTRUMENTS</t>
+  </si>
+  <si>
     <t>2496455</t>
   </si>
   <si>
@@ -1026,7 +1074,7 @@
     <t>http://www.ti.com/lit/ds/symlink/ne5532a.pdf</t>
   </si>
   <si>
-    <t>U4, U36</t>
+    <t>U4, U36, U?</t>
   </si>
   <si>
     <t>Quad Audio OpAmp</t>
@@ -1194,57 +1242,45 @@
     <t>http://www.farnell.com/datasheets/808691.pdf</t>
   </si>
   <si>
-    <t>U38</t>
-  </si>
-  <si>
-    <t>SN74LS14D</t>
-  </si>
-  <si>
-    <t>9592326</t>
+    <t>U38, U40, U44</t>
+  </si>
+  <si>
+    <t>Buffers &amp; Transmetteurs</t>
+  </si>
+  <si>
+    <t>SN74LVC1G07DCKR</t>
+  </si>
+  <si>
+    <t>1287544</t>
+  </si>
+  <si>
+    <t>DCK5</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn74lvc1g07.pdf</t>
+  </si>
+  <si>
+    <t>U39</t>
+  </si>
+  <si>
+    <t>16b I/O Expander</t>
+  </si>
+  <si>
+    <t>MCP23017-E/SO</t>
+  </si>
+  <si>
+    <t>MICROCHIP</t>
+  </si>
+  <si>
+    <t>1332087</t>
   </si>
   <si>
     <t>SO14NB</t>
   </si>
   <si>
-    <t>http://www.ti.com/lit/ds/symlink/sn74ls14.pdf</t>
-  </si>
-  <si>
-    <t>U39</t>
-  </si>
-  <si>
-    <t>16b I/O Expander</t>
-  </si>
-  <si>
-    <t>MCP23017-E/SO</t>
-  </si>
-  <si>
-    <t>MICROCHIP</t>
-  </si>
-  <si>
-    <t>1332087</t>
-  </si>
-  <si>
     <t>http://www.farnell.com/datasheets/12179.pdf</t>
   </si>
   <si>
-    <t>U40, U44</t>
-  </si>
-  <si>
-    <t>Buffers &amp; Transmetteurs</t>
-  </si>
-  <si>
-    <t>SN74LVC1G07DCKR</t>
-  </si>
-  <si>
-    <t>1287544</t>
-  </si>
-  <si>
-    <t>DCK5</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/sn74lvc1g07.pdf</t>
-  </si>
-  <si>
     <t>U41</t>
   </si>
   <si>
@@ -1398,7 +1434,7 @@
     <t>http://www.farnell.com/datasheets/74794.pdf</t>
   </si>
   <si>
-    <t>U?</t>
+    <t>U51</t>
   </si>
   <si>
     <t>Micro-contrôleur ATMEGA</t>
@@ -1413,12 +1449,12 @@
     <t>1972086</t>
   </si>
   <si>
-    <t>32A</t>
-  </si>
-  <si>
     <t>http://www.farnell.com/datasheets/2047852.pdf</t>
   </si>
   <si>
+    <t>U52</t>
+  </si>
+  <si>
     <t>LED_Controller</t>
   </si>
   <si>
@@ -1431,18 +1467,24 @@
     <t>2519520</t>
   </si>
   <si>
+    <t>U53</t>
+  </si>
+  <si>
     <t>8 ADC Package SPI</t>
   </si>
   <si>
-    <t>MCP3008-I/P</t>
-  </si>
-  <si>
-    <t>1627174</t>
+    <t>MCP3008-I/SL</t>
+  </si>
+  <si>
+    <t>1292241</t>
   </si>
   <si>
     <t>PDIP16_300MC</t>
   </si>
   <si>
+    <t>U54, U55, U56, U57</t>
+  </si>
+  <si>
     <t>Encodeurs cliquables</t>
   </si>
   <si>
@@ -1453,6 +1495,12 @@
   </si>
   <si>
     <t>2663521</t>
+  </si>
+  <si>
+    <t>U58</t>
+  </si>
+  <si>
+    <t>ZCZ324</t>
   </si>
   <si>
     <t>VR1, VR2</t>
@@ -1853,7 +1901,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1958,7 +2006,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>25</v>
@@ -1993,7 +2041,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>25</v>
@@ -2028,7 +2076,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>37</v>
@@ -2334,33 +2382,33 @@
         <v>86</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="3">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>85</v>
@@ -2369,182 +2417,182 @@
         <v>93</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3">
+        <v>76</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="3">
-        <v>30</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="3">
-        <v>78</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H18" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>121</v>
@@ -2553,226 +2601,226 @@
         <v>17</v>
       </c>
       <c r="H20" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="G21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="3">
+        <v>9</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="3">
-        <v>65</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="H26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2780,7 +2828,7 @@
         <v>154</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>155</v>
@@ -2801,313 +2849,313 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="3">
-        <v>3</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="G30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="3">
-        <v>4</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>185</v>
+        <v>128</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="H31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>187</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="3">
+        <v>4</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H34" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>117</v>
+        <v>208</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>17</v>
@@ -3116,33 +3164,33 @@
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>17</v>
@@ -3151,33 +3199,33 @@
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>224</v>
+        <v>128</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>227</v>
+        <v>128</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>17</v>
@@ -3186,33 +3234,33 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>231</v>
+        <v>128</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>15</v>
+        <v>229</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>17</v>
@@ -3221,150 +3269,150 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>117</v>
+        <v>231</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H40" s="3">
-        <v>86</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>249</v>
+        <v>128</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>241</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>117</v>
+        <v>244</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="H41" s="3">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>117</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="G42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42" s="3">
-        <v>54</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="G43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="3">
+        <v>85</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="3">
-        <v>34</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>261</v>
@@ -3378,136 +3426,136 @@
         <v>263</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" s="3">
+        <v>42</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H44" s="3">
-        <v>4</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="J44" s="2" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>255</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="3">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H46" s="3">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>275</v>
+        <v>111</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H47" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3518,156 +3566,156 @@
         <v>280</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>281</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H48" s="3">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>26</v>
+        <v>284</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>117</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H49" s="3">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>271</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H50" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H51" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>17</v>
@@ -3676,138 +3724,138 @@
         <v>4</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H53" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>253</v>
+        <v>307</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H54" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="G55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H55" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>255</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>17</v>
@@ -3816,68 +3864,68 @@
         <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="E57" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H57" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>17</v>
@@ -3886,74 +3934,74 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>259</v>
+        <v>111</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H59" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>309</v>
+        <v>111</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H60" s="3">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>311</v>
@@ -3962,272 +4010,272 @@
         <v>26</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C61" s="2" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>254</v>
+        <v>304</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H61" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>117</v>
+        <v>319</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>317</v>
+        <v>255</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H62" s="3">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>117</v>
+        <v>323</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>129</v>
+        <v>328</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H63" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>327</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H64" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>333</v>
+        <v>128</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>129</v>
+        <v>340</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H66" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>332</v>
+        <v>354</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H67" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>229</v>
+        <v>360</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>17</v>
@@ -4236,208 +4284,208 @@
         <v>3</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>117</v>
+        <v>362</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>336</v>
+        <v>365</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>331</v>
+        <v>140</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H69" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>362</v>
+        <v>243</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H70" s="3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>129</v>
+        <v>347</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H71" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>129</v>
+        <v>378</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H72" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>374</v>
+        <v>128</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H73" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>342</v>
+        <v>387</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>343</v>
+        <v>388</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>344</v>
+        <v>140</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>345</v>
+        <v>389</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>17</v>
@@ -4446,68 +4494,68 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>339</v>
+        <v>390</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>347</v>
+        <v>391</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>362</v>
+        <v>140</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H75" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>382</v>
+        <v>355</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>386</v>
+        <v>359</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>387</v>
+        <v>360</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>388</v>
+        <v>361</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>17</v>
@@ -4516,68 +4564,68 @@
         <v>1</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>389</v>
+        <v>355</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>390</v>
+        <v>363</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H77" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>17</v>
@@ -4586,68 +4634,68 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H79" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>331</v>
+        <v>416</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>17</v>
@@ -4656,103 +4704,103 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>417</v>
+        <v>347</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="H81" s="3">
         <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>117</v>
+        <v>424</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>17</v>
+        <v>199</v>
       </c>
       <c r="H82" s="3">
         <v>1</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>425</v>
+        <v>128</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>117</v>
+        <v>431</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>17</v>
@@ -4761,33 +4809,33 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>432</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>17</v>
@@ -4796,33 +4844,33 @@
         <v>1</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>331</v>
+        <v>448</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>17</v>
@@ -4831,33 +4879,33 @@
         <v>1</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>129</v>
+        <v>347</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>17</v>
@@ -4866,33 +4914,33 @@
         <v>1</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>455</v>
+        <v>140</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>17</v>
@@ -4901,33 +4949,33 @@
         <v>1</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>17</v>
@@ -4936,33 +4984,33 @@
         <v>1</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>17</v>
@@ -4971,33 +5019,33 @@
         <v>1</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>117</v>
+        <v>476</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>399</v>
+        <v>480</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>17</v>
@@ -5006,103 +5054,103 @@
         <v>1</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>473</v>
+        <v>128</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>459</v>
+        <v>482</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>476</v>
+        <v>416</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H91" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>117</v>
+        <v>486</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>331</v>
+        <v>490</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H92" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>482</v>
+        <v>128</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>483</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>479</v>
+        <v>421</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>485</v>
+        <v>422</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>486</v>
+        <v>347</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>487</v>
+        <v>423</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>17</v>
@@ -5111,48 +5159,118 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>489</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>479</v>
+        <v>495</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>399</v>
+        <v>347</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H94" s="3">
+        <v>2</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="3">
         <v>1</v>
       </c>
-      <c r="I94" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K94" s="2" t="s">
-        <v>494</v>
+      <c r="I95" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96" s="3">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final components and set deceitful footprints
</commit_message>
<xml_diff>
--- a/Bill of Materials-Michel.xlsx
+++ b/Bill of Materials-Michel.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocal\Desktop\electronic-levelup-hardware\Michel\Project Outputs for Michel\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24015" windowHeight="15825"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="548">
   <si>
     <t>Designator</t>
   </si>
@@ -54,7 +59,7 @@
     <t>DataSheet</t>
   </si>
   <si>
-    <t>C1, C4, C140, C157, C158, C159, C160, C166, C167, C168, C169, C172, C173, C175_Audio Input L, C175_Audio Input R, C175_Audio Repeat L, C175_Audio Repeat R, C191, C196, C205, C210, C261_Mode Select 1A, C261_Mode Select 1B, C261_Mode Select 2A, C261_Mode Select 2B, C288, C291, C292, C295</t>
+    <t>C1, C4, C139, C157, C158, C159, C160, C166, C169, C170, C171, C172, C173, C176_Audio Input L, C176_Audio Input R, C176_Audio Repeat L, C176_Audio Repeat R, C191, C196, C205, C210, C261_Mode Select 1A, C261_Mode Select 1B, C261_Mode Select 2A, C261_Mode Select 2B, C288, C289, C290, C291</t>
   </si>
   <si>
     <t>10uF</t>
@@ -159,25 +164,25 @@
     <t>http://www.farnell.com/datasheets/2048127.pdf</t>
   </si>
   <si>
-    <t>C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C61, C136, C137, C139, C141, C142, C143, C144, C145, C146, C147, C148, C149, C150, C151, C152, C153, C154, C155</t>
-  </si>
-  <si>
-    <t>22uF, 100nF, 10uF, 22uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 2.2uF, 10uF, 2.2uF, 4.7uF, 4.7uF, 10uF, 10uF, 10uF, 22uF, 4.7uF, 0.1uF, 10uF, 0.1uF, 0.1uF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF</t>
+    <t>C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C61, C136, C137, C140, C141, C142, C143, C144, C145, C146, C147, C148, C149, C150, C151, C152, C153, C154, C155</t>
+  </si>
+  <si>
+    <t>22uF, 100nF, 10uF, 22uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 10uF, 2.2uF, 10uF, 2.2uF, 4.7uF, 4.7uF, 10uF, 10uF, 10uF, 22uF, 4.7uF, 10uF, 0.1uF, 0.1uF, 0.1uF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF, 100nF</t>
   </si>
   <si>
     <t>Capacitor</t>
   </si>
   <si>
-    <t>GRM188R60J226MEA0D, GRM188F51E104ZA01D, GRM188R60J106ME47J, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J475KE19D, GRM188R60J475KE19D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, ZRB18AR60J226ME01L, GRM188R60J475KE19D, GRM188F51E104ZA01D, GRM188R60J106ME47J, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D</t>
-  </si>
-  <si>
-    <t>2666490, 1828902, 2611921, 2666490, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2672153, 2611921, 2672153, 2666491, 2666491, 2611921, 2611921, 2611921, 2666613, 2666491, 2821272, 2611921, 2821272, 2821272, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2163235.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf</t>
-  </si>
-  <si>
-    <t>C32, C34, C35, C38, C39, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C62, C68, C69, C70, C72, C73, C74, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C97, C98, C99, C100, C101, C102, C107, C108, C109, C110, C111, C112, C113, C114, C116, C117, C118, C119, C120, C121, C122, C123, C124, C129, C130, C131, C132, C133</t>
+    <t>GRM188R60J226MEA0D, GRM188F51E104ZA01D, GRM188R60J106ME47J, GRM188R60J226MEA0D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J106ME47J, GRT188R60J225KE13D, GRM188R60J475KE19D, GRM188R60J475KE19D, GRM188R60J106ME47J, GRM188R60J106ME47J, GRM188R60J106ME47J, ZRB18AR60J226ME01L, GRM188R60J475KE19D, GRM188R60J106ME47J, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D, GRM188F51E104ZA01D</t>
+  </si>
+  <si>
+    <t>2666490, 1828902, 2611921, 2666490, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2611921, 2672153, 2611921, 2672153, 2666491, 2666491, 2611921, 2611921, 2611921, 2666613, 2666491, 2611921, 2821272, 2821272, 2821272, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902, 1828902</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/1955681.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2165952.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2163235.pdf, http://www.farnell.com/datasheets/2048798.pdf, http://www.farnell.com/datasheets/2079165.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf, http://www.farnell.com/datasheets/2048672.pdf</t>
+  </si>
+  <si>
+    <t>C32, C34, C35, C38, C39, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56, C62, C68, C69, C70, C72, C73, C74, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C97, C98, C99, C100, C101, C102, C107, C108, C109, C110, C111, C112, C113, C115, C116, C117, C118, C119, C120, C121, C122, C123, C124, C129, C130, C131, C132, C133</t>
   </si>
   <si>
     <t>100pF</t>
@@ -270,7 +275,7 @@
     <t>http://www.farnell.com/datasheets/2048220.pdf</t>
   </si>
   <si>
-    <t>C71, C103, C115, C125, C134</t>
+    <t>C71, C103, C114, C125, C134</t>
   </si>
   <si>
     <t>GRM155R61A224KE19D</t>
@@ -294,7 +299,7 @@
     <t>http://www.farnell.com/datasheets/2165911.pdf</t>
   </si>
   <si>
-    <t>C135, C138, C178_Audio Input L, C178_Audio Input R, C178_Audio Repeat L, C178_Audio Repeat R, C179_Audio Input L, C179_Audio Input R, C179_Audio Repeat L, C179_Audio Repeat R, C180_Audio Input L, C180_Audio Input R, C180_Audio Repeat L, C180_Audio Repeat R, C187_Audio Output1, C187_Audio Output2, C187_Audio Output3, C188_Audio Output1, C188_Audio Output2, C188_Audio Output3, C198, C199, C200, C201, C202, C214_MS - LR Converter1, C214_MS - LR Converter2, C215_MS - LR Converter1, C215_MS - LR Converter2, C216_MS - LR Converter1, C216_MS - LR Converter2, C217_MS - LR Converter1, C217_MS - LR Converter2, C218_MS - LR Converter1, C218_MS - LR Converter2, C223, C224, C225, C226, C233, C234, C235, C242, C243, C250, C251, C252, C259, C260, C262_Mode Select 1A, C262_Mode Select 1B, C262_Mode Select 2A, C262_Mode Select 2B, C263, C264, C265, C266, C267, C268, C269, C270, C271, C272, C273, C282, C283, C284, C285, C286, C287, C289, C290, C293, C294</t>
+    <t>C135, C138, C178_Audio Input L, C178_Audio Input R, C178_Audio Repeat L, C178_Audio Repeat R, C179_Audio Input L, C179_Audio Input R, C179_Audio Repeat L, C179_Audio Repeat R, C180_Audio Input L, C180_Audio Input R, C180_Audio Repeat L, C180_Audio Repeat R, C187_Audio Output1, C187_Audio Output2, C187_Audio Output3, C188_Audio Output1, C188_Audio Output2, C188_Audio Output3, C198, C199, C200, C201, C202, C214_MS - LR Converter1, C214_MS - LR Converter2, C215_MS - LR Converter1, C215_MS - LR Converter2, C216_MS - LR Converter1, C216_MS - LR Converter2, C217_MS - LR Converter1, C217_MS - LR Converter2, C218_MS - LR Converter1, C218_MS - LR Converter2, C223, C224, C225, C226, C233, C234, C235, C242, C243, C250, C251, C252, C259, C260, C262_Mode Select 1A, C262_Mode Select 1B, C262_Mode Select 2A, C262_Mode Select 2B, C263, C264, C265, C266, C267, C268, C269, C270, C271, C272, C273, C282, C283, C284, C285, C286, C287, C292, C293, C294, C295</t>
   </si>
   <si>
     <t>GRM188F51E104ZA01D</t>
@@ -306,7 +311,7 @@
     <t>http://www.farnell.com/datasheets/2048672.pdf</t>
   </si>
   <si>
-    <t>C156, C161, C162, C163, C164, C165, C170, C171, C176_Audio Input L, C176_Audio Input R, C176_Audio Repeat L, C176_Audio Repeat R, C177_Audio Input L, C177_Audio Input R, C177_Audio Repeat L, C177_Audio Repeat R, C181_Audio Output1, C181_Audio Output2, C181_Audio Output3, C182_Audio Output1, C182_Audio Output2, C182_Audio Output3, C183_Audio Output1, C183_Audio Output2, C183_Audio Output3, C184_Audio Output1, C184_Audio Output2, C184_Audio Output3, C185_Audio Output1, C185_Audio Output2, C185_Audio Output3, C186_Audio Output1, C186_Audio Output2, C186_Audio Output3</t>
+    <t>C156, C161, C162, C163, C164, C165, C167, C168, C175_Audio Input L, C175_Audio Input R, C175_Audio Repeat L, C175_Audio Repeat R, C177_Audio Input L, C177_Audio Input R, C177_Audio Repeat L, C177_Audio Repeat R, C181_Audio Output1, C181_Audio Output2, C181_Audio Output3, C182_Audio Output1, C182_Audio Output2, C182_Audio Output3, C183_Audio Output1, C183_Audio Output2, C183_Audio Output3, C184_Audio Output1, C184_Audio Output2, C184_Audio Output3, C185_Audio Output1, C185_Audio Output2, C185_Audio Output3, C186_Audio Output1, C186_Audio Output2, C186_Audio Output3</t>
   </si>
   <si>
     <t>1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 1uF, 0.01uF, 0.01uF, 0.01uF, 0.01uF, 2200pF, 2200pF, 2200pF, 2200pF, 330pF, 330pF, 330pF, 1500pF, 1500pF, 1500pF, 330pF, 330pF, 330pF, 330pF, 330pF, 330pF, 1500pF, 1500pF, 1500pF, 330pF, 330pF, 330pF</t>
@@ -564,31 +569,49 @@
     <t>http://www.farnell.com/datasheets/866888.pdf</t>
   </si>
   <si>
-    <t>L1, L2, L3, L4</t>
-  </si>
-  <si>
-    <t>2.2uH, 2.2uH, 2.2uH, 18uH</t>
+    <t>L1, L2, L3</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
   </si>
   <si>
     <t>Inductor</t>
   </si>
   <si>
-    <t>3613C220K, 3613C220K, 3613C220K, MLF2012C180K</t>
-  </si>
-  <si>
-    <t>SIGMAINDUCTORS - TE CONNECTIVITY, SIGMAINDUCTORS - TE CONNECTIVITY, SIGMAINDUCTORS - TE CONNECTIVITY, TDK</t>
-  </si>
-  <si>
-    <t>1174074, 1174074, 1174074, 1669551</t>
-  </si>
-  <si>
-    <t>0402-A</t>
-  </si>
-  <si>
-    <t>1812 [4532 Metric], 1812 [4532 Metric], 1812 [4532 Metric], 0805 [2012 Metric]</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/cad/1576322.pdf, http://www.farnell.com/datasheets/321059.pdf</t>
+    <t>LQM18NN2R2K00D</t>
+  </si>
+  <si>
+    <t>1343118</t>
+  </si>
+  <si>
+    <t>INDM1608X08N</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/66032.pdf</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>18uH</t>
+  </si>
+  <si>
+    <t>MLF2012C180K</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>1669551</t>
+  </si>
+  <si>
+    <t>INDM2612X12N</t>
+  </si>
+  <si>
+    <t>0805 [2012 Metric]</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/321059.pdf</t>
   </si>
   <si>
     <t>L5, L6, L7</t>
@@ -606,7 +629,7 @@
     <t>1515495</t>
   </si>
   <si>
-    <t>6-0805_M</t>
+    <t>INDM5750X47N</t>
   </si>
   <si>
     <t>2220 [5650 Metric]</t>
@@ -669,7 +692,70 @@
     <t>http://www.farnell.com/datasheets/1912447.pdf</t>
   </si>
   <si>
-    <t>P4, P5</t>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>Header, 3-Pin</t>
+  </si>
+  <si>
+    <t>1241150-3</t>
+  </si>
+  <si>
+    <t>2399724</t>
+  </si>
+  <si>
+    <t>CONN_1241150-3_T</t>
+  </si>
+  <si>
+    <t>P5, P7</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P8, P9</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>RK09K1130C79</t>
+  </si>
+  <si>
+    <t>ALPS</t>
+  </si>
+  <si>
+    <t>1191741</t>
+  </si>
+  <si>
+    <t>ALPS_RK09K1130C79</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2160634.pdf</t>
+  </si>
+  <si>
+    <t>P10, P11, P12, P13</t>
+  </si>
+  <si>
+    <t>P160KMP-0QC20B10K</t>
+  </si>
+  <si>
+    <t>Bi Technology</t>
+  </si>
+  <si>
+    <t>1760793</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2331843.pdf</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15, P16</t>
   </si>
   <si>
     <t>DIN 5pin</t>
@@ -690,30 +776,6 @@
     <t>http://www.farnell.com/datasheets/1697491.pdf</t>
   </si>
   <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>Header, 3-Pin</t>
-  </si>
-  <si>
-    <t>1241150-3</t>
-  </si>
-  <si>
-    <t>2399724</t>
-  </si>
-  <si>
-    <t>CONN_1241150-3_T</t>
-  </si>
-  <si>
-    <t>P7, P9</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -726,6 +788,9 @@
     <t>2467855</t>
   </si>
   <si>
+    <t>SON440P360X120-4N</t>
+  </si>
+  <si>
     <t>http://www.farnell.com/datasheets/1750519.pdf</t>
   </si>
   <si>
@@ -747,7 +812,7 @@
     <t>9713220</t>
   </si>
   <si>
-    <t>R38</t>
+    <t>SON550P380X250-4N</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2175893.pdf</t>
@@ -807,7 +872,7 @@
     <t>http://www.farnell.com/datasheets/19296.pdf</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R72, R73, R74, R75, R76, R77, R78, R79, R80, R81, R103, R104, R105, R106, R107, R108, R109, R110, R111, R112, R113, R114, R115, R116, R117, R118, R119, R120, R121, R122, R123, R124, R125, R126, R201, R202, R203_Audio Input L, R203_Audio Input R, R203_Audio Repeat L, R203_Audio Repeat R, R204_Audio Input L, R204_Audio Input R, R204_Audio Repeat L, R204_Audio Repeat R, R205_Audio Input L, R205_Audio Input R, R205_Audio Repeat L, R205_Audio Repeat R, R206_Audio Input L, R206_Audio Input R, R206_Audio Repeat L, R206_Audio Repeat R, R207_Audio Input L, R207_Audio Input R, R207_Audio Repeat L, R207_Audio Repeat R, R208_Audio Input L, R208_Audio Input R, R208_Audio Repeat L, R208_Audio Repeat R, R209_Audio Output1, R209_Audio Output2, R209_Audio Output3, R210_Audio Output1, R210_Audio Output2, R210_Audio Output3, R211_Audio Output1, R211_Audio Output2, R211_Audio Output3, R212_Audio Output1, R212_Audio Output2, R212_Audio Output3, R213_Audio Output1, R213_Audio Output2, R213_Audio Output3, R214_Audio Output1, R214_Audio Output2, R214_Audio Output3, R215_Audio Output1, R215_Audio Output2, R215_Audio Output3, R216_Audio Output1, R216_Audio Output2, R216_Audio Output3, R217_Audio Output1, R217_Audio Output2, R217_Audio Output3, R218_Audio Output1, R218_Audio Output2, R218_Audio Output3, R219_Audio Output1, R219_Audio Output2, R219_Audio Output3, R220_Audio Output1, R220_Audio Output2, R220_Audio Output3, R221_Audio Output1, R221_Audio Output2, R221_Audio Output3, R222_Audio Output1, R222_Audio Output2, R222_Audio Output3, R400, R401, R402, R403, R404, R405, R406, R407, R409, R412, R415, R418</t>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R72, R73, R74, R75, R76, R77, R78, R79, R80, R81, R103, R104, R105, R106, R107, R108, R109, R110, R111, R112, R113, R114, R115, R116, R117, R118, R119, R120, R121, R122, R123, R124, R125, R126, R195, R196, R197_Audio Input L, R197_Audio Input R, R197_Audio Repeat L, R197_Audio Repeat R, R198_Audio Input L, R198_Audio Input R, R198_Audio Repeat L, R198_Audio Repeat R, R199_Audio Input L, R199_Audio Input R, R199_Audio Repeat L, R199_Audio Repeat R, R200_Audio Input L, R200_Audio Input R, R200_Audio Repeat L, R200_Audio Repeat R, R201_Audio Input L, R201_Audio Input R, R201_Audio Repeat L, R201_Audio Repeat R, R202_Audio Input L, R202_Audio Input R, R202_Audio Repeat L, R202_Audio Repeat R, R203_Audio Output1, R203_Audio Output2, R203_Audio Output3, R204_Audio Output1, R204_Audio Output2, R204_Audio Output3, R205_Audio Output1, R205_Audio Output2, R205_Audio Output3, R206_Audio Output1, R206_Audio Output2, R206_Audio Output3, R207_Audio Output1, R207_Audio Output2, R207_Audio Output3, R208_Audio Output1, R208_Audio Output2, R208_Audio Output3, R209_Audio Output1, R209_Audio Output2, R209_Audio Output3, R210_Audio Output1, R210_Audio Output2, R210_Audio Output3, R211_Audio Output1, R211_Audio Output2, R211_Audio Output3, R212_Audio Output1, R212_Audio Output2, R212_Audio Output3, R213_Audio Output1, R213_Audio Output2, R213_Audio Output3, R214_Audio Output1, R214_Audio Output2, R214_Audio Output3, R215_Audio Output1, R215_Audio Output2, R215_Audio Output3, R216_Audio Output1, R216_Audio Output2, R216_Audio Output3, R394, R395, R396, R397, R398, R399, R400, R401, R403, R406, R409, R412</t>
   </si>
   <si>
     <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, DNI, 0, 0, DNI, 0, 0, 0, 0, 0, 0, 0, 0, DNI, 0, 0, DNI, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, DNI, DNI, DNI, DNI, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 10k, 10k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 1.5k, 1.5k, 1.5k, 1.5k, 3k, 3k, 3k, 3k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 10k, 20k, 10k, 20k, 10k, 20k, 10k, 20k, 0, 0, 0, 0</t>
@@ -828,13 +893,13 @@
     <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, [NoParam], [NoParam], [NoParam], [NoParam]</t>
   </si>
   <si>
-    <t>R82, R83, R84, R85, R235, R236, R237, R266_MS - LR Converter1, R266_MS - LR Converter2, R267_MS - LR Converter1, R267_MS - LR Converter2, R268, R272, R296, R297, R298, R339, R340, R341, R363_Mode Select 1A, R363_Mode Select 1B, R363_Mode Select 2A, R363_Mode Select 2B, R364_Mode Select 1A, R364_Mode Select 1B, R364_Mode Select 2A, R364_Mode Select 2B, R365_Mode Select 1A, R365_Mode Select 1B, R365_Mode Select 2A, R365_Mode Select 2B, R366, R367, R377, R378, R379, R394, R395, R396, R397, R398, R399</t>
+    <t>R82, R83, R84, R85, R229, R230, R231, R260_MS - LR Converter1, R260_MS - LR Converter2, R261_MS - LR Converter1, R261_MS - LR Converter2, R262, R266, R290, R291, R292, R333, R334, R335, R357_Mode Select 1A, R357_Mode Select 1B, R357_Mode Select 2A, R357_Mode Select 2B, R358_Mode Select 1A, R358_Mode Select 1B, R358_Mode Select 2A, R358_Mode Select 2B, R359_Mode Select 1A, R359_Mode Select 1B, R359_Mode Select 2A, R359_Mode Select 2B, R360, R361, R371, R372, R373, R388, R389, R390, R391, R392, R393</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>R86, R87, R88, R89, R90, R91, R92, R93, R94, R128, R129, R130, R131, R132, R133, R134, R135, R136, R137, R138, R139, R140, R141, R142, R143, R144, R145, R146, R147, R148, R149, R150, R151, R152, R153, R154, R155, R156, R157, R158, R159, R160, R161, R162, R163, R164, R165, R166, R167, R168, R169, R177, R178, R179, R180, R181, R182, R183, R184, R185, R186, R187, R188, R189, R190, R191, R192, R193, R194, R195, R196, R197, R198, R199, R200</t>
+    <t>R86, R87, R88, R89, R90, R91, R92, R93, R94, R128, R129, R130, R131, R132, R133, R134, R135, R136, R137, R138, R139, R140, R141, R142, R143, R144, R145, R146, R147, R148, R149, R150, R151, R152, R153, R154, R155, R156, R157, R158, R159, R160, R161, R162, R163, R164, R165, R166, R167, R168, R169, R171, R172, R173, R174, R175, R176, R177, R178, R179, R180, R181, R182, R183, R184, R185, R186, R187, R188, R189, R190, R191, R192, R193, R194</t>
   </si>
   <si>
     <t>0, 0, 10k, 10k, 100k, 100k, 0, 0, 10k, 1.2k, 0, DNI, 10k, DNI, DNI, 100K, DNI, DNI, DNI, DNI, DNI, DNI, 100K, DNI, DNI, DNI, DNI, 100K, DNI, 100K, 100K, DNI, 100K, 100K, 100K, 100K, 100K, 100K, DNI, 100K, 100K, 100K, 100K, DNI, 100K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k</t>
@@ -852,9 +917,6 @@
     <t>R95</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>CPF-A-0603B4K7E1</t>
   </si>
   <si>
@@ -879,7 +941,7 @@
     <t>R98</t>
   </si>
   <si>
-    <t>R99, R100, R127, R223, R224, R225, R227, R229, R231, R232, R234, R238, R239, R240, R242, R244, R246, R247, R249, R250_MS - LR Converter1, R250_MS - LR Converter2, R251_MS - LR Converter1, R251_MS - LR Converter2, R252_MS - LR Converter1, R252_MS - LR Converter2, R253_MS - LR Converter1, R253_MS - LR Converter2, R254_MS - LR Converter1, R254_MS - LR Converter2, R255_MS - LR Converter1, R255_MS - LR Converter2, R257_MS - LR Converter1, R257_MS - LR Converter2, R258_MS - LR Converter1, R258_MS - LR Converter2, R259_MS - LR Converter1, R259_MS - LR Converter2, R260_MS - LR Converter1, R260_MS - LR Converter2, R261_MS - LR Converter1, R261_MS - LR Converter2, R262_MS - LR Converter1, R262_MS - LR Converter2, R263_MS - LR Converter1, R263_MS - LR Converter2, R264_MS - LR Converter1, R264_MS - LR Converter2, R270, R274, R372, R373, R384, R385</t>
+    <t>R99, R100, R127, R217, R218, R219, R221, R223, R225, R226, R228, R232, R233, R234, R236, R238, R240, R241, R243, R244_MS - LR Converter1, R244_MS - LR Converter2, R245_MS - LR Converter1, R245_MS - LR Converter2, R246_MS - LR Converter1, R246_MS - LR Converter2, R247_MS - LR Converter1, R247_MS - LR Converter2, R248_MS - LR Converter1, R248_MS - LR Converter2, R249_MS - LR Converter1, R249_MS - LR Converter2, R251_MS - LR Converter1, R251_MS - LR Converter2, R252_MS - LR Converter1, R252_MS - LR Converter2, R253_MS - LR Converter1, R253_MS - LR Converter2, R254_MS - LR Converter1, R254_MS - LR Converter2, R255_MS - LR Converter1, R255_MS - LR Converter2, R256_MS - LR Converter1, R256_MS - LR Converter2, R257_MS - LR Converter1, R257_MS - LR Converter2, R258_MS - LR Converter1, R258_MS - LR Converter2, R264, R268, R366, R367, R378, R379</t>
   </si>
   <si>
     <t>1K, 1K, 1K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k</t>
@@ -897,25 +959,7 @@
     <t>R102</t>
   </si>
   <si>
-    <t>R170, R171, R172, R173, R174, R175</t>
-  </si>
-  <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>RK09K1130C79, RK09K1130C79, P160KMP-0QC20B10K, P160KMP-0QC20B10K, P160KMP-0QC20B10K, P160KMP-0QC20B10K</t>
-  </si>
-  <si>
-    <t>ALPS, ALPS, Bi Technology, Bi Technology, Bi Technology, Bi Technology</t>
-  </si>
-  <si>
-    <t>1191741, 1191741, 1760793, 1760793, 1760793, 1760793</t>
-  </si>
-  <si>
-    <t>VR5</t>
-  </si>
-  <si>
-    <t>R176, R279, R280, R281, R282, R283, R284, R287, R292, R302, R303, R304, R305, R306, R307, R310, R315, R322, R323, R324, R325, R326, R327, R330, R335, R345, R346, R347, R348, R349, R350, R353, R358</t>
+    <t>R170, R273, R274, R275, R276, R277, R278, R281, R286, R296, R297, R298, R299, R300, R301, R304, R309, R316, R317, R318, R319, R320, R321, R324, R329, R339, R340, R341, R342, R343, R344, R347, R352</t>
   </si>
   <si>
     <t>33k</t>
@@ -927,7 +971,7 @@
     <t>2483920</t>
   </si>
   <si>
-    <t>R226, R228, R233, R241, R243, R248, R256_MS - LR Converter1, R256_MS - LR Converter2, R265_MS - LR Converter1, R265_MS - LR Converter2, R269, R273, R276, R277, R278, R293, R295, R299, R300, R301, R316, R318, R319, R320, R321, R336, R338, R342, R343, R344, R359, R361, R370, R371, R376, R382, R383, R388</t>
+    <t>R220, R222, R227, R235, R237, R242, R250_MS - LR Converter1, R250_MS - LR Converter2, R259_MS - LR Converter1, R259_MS - LR Converter2, R263, R267, R270, R271, R272, R287, R289, R293, R294, R295, R310, R312, R313, R314, R315, R330, R332, R336, R337, R338, R353, R355, R364, R365, R370, R376, R377, R382</t>
   </si>
   <si>
     <t>100k</t>
@@ -942,7 +986,7 @@
     <t>http://www.farnell.com/datasheets/2189072.pdf</t>
   </si>
   <si>
-    <t>R230, R245, R389, R392, R393</t>
+    <t>R224, R239, R383, R386, R387</t>
   </si>
   <si>
     <t>220k</t>
@@ -954,7 +998,7 @@
     <t>2483903</t>
   </si>
   <si>
-    <t>R271, R275</t>
+    <t>R265, R269</t>
   </si>
   <si>
     <t>13k</t>
@@ -969,13 +1013,13 @@
     <t>http://www.farnell.com/datasheets/2104089.pdf</t>
   </si>
   <si>
-    <t>R285, R286, R294, R308, R309, R317, R328, R329, R337, R351, R352, R360, R368, R380, R391, R408, R410, R411, R413, R414, R416, R417, R419</t>
+    <t>R279, R280, R288, R302, R303, R311, R322, R323, R331, R345, R346, R354, R362, R374, R385, R402, R404, R405, R407, R408, R410, R411, R413</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>R288, R289, R311, R312, R331, R332, R354, R355</t>
+    <t>R282, R283, R305, R306, R325, R326, R348, R349</t>
   </si>
   <si>
     <t>51k</t>
@@ -990,13 +1034,13 @@
     <t>http://www.farnell.com/datasheets/2043335.pdf</t>
   </si>
   <si>
-    <t>R290, R291, R313, R314, R333, R334, R356, R357, R375, R387</t>
+    <t>R284, R285, R307, R308, R327, R328, R350, R351, R369, R381</t>
   </si>
   <si>
     <t>4.7k</t>
   </si>
   <si>
-    <t>R362_Mode Select 1A, R362_Mode Select 1B, R362_Mode Select 2A, R362_Mode Select 2B</t>
+    <t>R356_Mode Select 1A, R356_Mode Select 1B, R356_Mode Select 2A, R356_Mode Select 2B</t>
   </si>
   <si>
     <t>470k</t>
@@ -1008,7 +1052,7 @@
     <t>2331232</t>
   </si>
   <si>
-    <t>R369, R374, R381, R386</t>
+    <t>R363, R368, R375, R380</t>
   </si>
   <si>
     <t>150k</t>
@@ -1020,10 +1064,31 @@
     <t>2330937</t>
   </si>
   <si>
-    <t>R390</t>
-  </si>
-  <si>
-    <t>S1, S2, S3</t>
+    <t>R384</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SPDT Subminiature Toggle Switch, Right Angle Mounting, Vertical Actuation</t>
+  </si>
+  <si>
+    <t>TS01ABE</t>
+  </si>
+  <si>
+    <t>C &amp; K COMPONENTS</t>
+  </si>
+  <si>
+    <t>2435185</t>
+  </si>
+  <si>
+    <t>C&amp;K_TS01ABE</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1839865.pdf</t>
+  </si>
+  <si>
+    <t>S2, S3, S4</t>
   </si>
   <si>
     <t>Commutateur tactile</t>
@@ -1032,9 +1097,6 @@
     <t>KMR211G LFS</t>
   </si>
   <si>
-    <t>C &amp; K COMPONENTS</t>
-  </si>
-  <si>
     <t>1437635</t>
   </si>
   <si>
@@ -1044,24 +1106,6 @@
     <t>http://www.farnell.com/datasheets/2044619.pdf</t>
   </si>
   <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>SPDT Subminiature Toggle Switch, Right Angle Mounting, Vertical Actuation</t>
-  </si>
-  <si>
-    <t>TS01ABE</t>
-  </si>
-  <si>
-    <t>2435185</t>
-  </si>
-  <si>
-    <t>C&amp;K_TS01ABE</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1839865.pdf</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -1080,7 +1124,7 @@
     <t>http://www.ti.com/lit/ds/symlink/tps65217.pdf</t>
   </si>
   <si>
-    <t>U2, U6, U58</t>
+    <t>U2, U6, U54</t>
   </si>
   <si>
     <t>Buffers &amp; Transmetteurs</t>
@@ -1224,6 +1268,27 @@
     <t>U10</t>
   </si>
   <si>
+    <t>8 ADC Package SPI</t>
+  </si>
+  <si>
+    <t>MCP3008-I/SL</t>
+  </si>
+  <si>
+    <t>MICROCHIP</t>
+  </si>
+  <si>
+    <t>1292241</t>
+  </si>
+  <si>
+    <t>PDIP16_300MC</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/808965.pdf</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
     <t>Micro-contrôleur ATMEGA</t>
   </si>
   <si>
@@ -1242,7 +1307,7 @@
     <t>http://www.farnell.com/datasheets/2047852.pdf</t>
   </si>
   <si>
-    <t>U11</t>
+    <t>U12</t>
   </si>
   <si>
     <t>LED_Controller</t>
@@ -1263,28 +1328,7 @@
     <t>http://www.farnell.com/datasheets/1825883.pdf</t>
   </si>
   <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>8 ADC Package SPI</t>
-  </si>
-  <si>
-    <t>MCP3008-I/SL</t>
-  </si>
-  <si>
-    <t>MICROCHIP</t>
-  </si>
-  <si>
-    <t>1292241</t>
-  </si>
-  <si>
-    <t>PDIP16_300MC</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/808965.pdf</t>
-  </si>
-  <si>
-    <t>U17, U18, U19, U20</t>
+    <t>U13, U14, U15, U16</t>
   </si>
   <si>
     <t>Encodeurs cliquables</t>
@@ -1299,7 +1343,13 @@
     <t>2663521</t>
   </si>
   <si>
-    <t>U21</t>
+    <t>BOURNS_PEC11R-4120F-S0018</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2360546.pdf</t>
+  </si>
+  <si>
+    <t>U17</t>
   </si>
   <si>
     <t>Codec Audio, 6ADC/8DAC</t>
@@ -1320,7 +1370,7 @@
     <t>http://www.ti.com/lit/ds/symlink/pcm3168a.pdf</t>
   </si>
   <si>
-    <t>U22_Audio Input L, U22_Audio Input R, U22_Audio Repeat L, U22_Audio Repeat R, U23_Audio Output1, U23_Audio Output2, U23_Audio Output3</t>
+    <t>U18_Audio Input L, U18_Audio Input R, U18_Audio Repeat L, U18_Audio Repeat R, U19_Audio Output1, U19_Audio Output2, U19_Audio Output3</t>
   </si>
   <si>
     <t>Amplificateur Opérationnel</t>
@@ -1338,7 +1388,7 @@
     <t>http://www.ti.com/lit/ds/symlink/ne5532a.pdf</t>
   </si>
   <si>
-    <t>U24, U56</t>
+    <t>U20, U52</t>
   </si>
   <si>
     <t>Quad Audio OpAmp</t>
@@ -1356,7 +1406,7 @@
     <t>http://www.ti.com/lit/ds/symlink/opa1654.pdf</t>
   </si>
   <si>
-    <t>U25, U35, U55</t>
+    <t>U21, U31, U51</t>
   </si>
   <si>
     <t>Dual DigiPot non volatile I2C</t>
@@ -1377,13 +1427,13 @@
     <t>http://www.farnell.com/datasheets/2243913.pdf</t>
   </si>
   <si>
-    <t>U26, U29_MS - LR Converter1, U29_MS - LR Converter2, U31</t>
+    <t>U22, U25_MS - LR Converter1, U25_MS - LR Converter2, U27</t>
   </si>
   <si>
     <t>Dual Audio OpAmp</t>
   </si>
   <si>
-    <t>U27_MS - LR Converter1, U27_MS - LR Converter2, U46</t>
+    <t>U23_MS - LR Converter1, U23_MS - LR Converter2, U42</t>
   </si>
   <si>
     <t>Quad 2:1 Multiplexer</t>
@@ -1401,7 +1451,7 @@
     <t>http://www.farnell.com/datasheets/2299862.pdf</t>
   </si>
   <si>
-    <t>U28_MS - LR Converter1, U28_MS - LR Converter2, U60</t>
+    <t>U24_MS - LR Converter1, U24_MS - LR Converter2, U56</t>
   </si>
   <si>
     <t>TL084ID</t>
@@ -1413,7 +1463,7 @@
     <t>http://www.ti.com/lit/ds/symlink/tl084.pdf</t>
   </si>
   <si>
-    <t>U30, U32, U44, U45, U47, U48, U49, U50, U51, U52, U53, U54</t>
+    <t>U26, U28, U40, U41, U43, U44, U45, U46, U47, U48, U49, U50</t>
   </si>
   <si>
     <t>Single 2:1 Multiplexer</t>
@@ -1431,7 +1481,7 @@
     <t>http://www.farnell.com/datasheets/2053574.pdf</t>
   </si>
   <si>
-    <t>U33, U36, U38, U41</t>
+    <t>U29, U32, U34, U37</t>
   </si>
   <si>
     <t>Hex Inverter</t>
@@ -1446,7 +1496,7 @@
     <t>http://www.ti.com/lit/ds/symlink/cd4069ub.pdf</t>
   </si>
   <si>
-    <t>U34</t>
+    <t>U30</t>
   </si>
   <si>
     <t>Dual Transconductance OpAmp</t>
@@ -1464,13 +1514,13 @@
     <t>http://www.ti.com/lit/ds/symlink/lm13700.pdf</t>
   </si>
   <si>
-    <t>U37, U39, U42</t>
-  </si>
-  <si>
-    <t>U40</t>
-  </si>
-  <si>
-    <t>U43_Mode Select 1A, U43_Mode Select 1B, U43_Mode Select 2A, U43_Mode Select 2B</t>
+    <t>U33, U35, U38</t>
+  </si>
+  <si>
+    <t>U36</t>
+  </si>
+  <si>
+    <t>U39_Mode Select 1A, U39_Mode Select 1B, U39_Mode Select 2A, U39_Mode Select 2B</t>
   </si>
   <si>
     <t>Dual 4:1 Multiplexer</t>
@@ -1488,48 +1538,48 @@
     <t>http://www.farnell.com/datasheets/2051461.pdf</t>
   </si>
   <si>
+    <t>U53</t>
+  </si>
+  <si>
+    <t>Optocoupler</t>
+  </si>
+  <si>
+    <t>6N139</t>
+  </si>
+  <si>
+    <t>TOSHIBA</t>
+  </si>
+  <si>
+    <t>1225823</t>
+  </si>
+  <si>
+    <t>DIP8_VISHAY_6N13</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/808691.pdf</t>
+  </si>
+  <si>
+    <t>U55</t>
+  </si>
+  <si>
+    <t>16b I/O Expander</t>
+  </si>
+  <si>
+    <t>MCP23017-E/SO</t>
+  </si>
+  <si>
+    <t>1332087</t>
+  </si>
+  <si>
+    <t>SO14NB</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/12179.pdf</t>
+  </si>
+  <si>
     <t>U57</t>
   </si>
   <si>
-    <t>Optocoupler</t>
-  </si>
-  <si>
-    <t>6N139</t>
-  </si>
-  <si>
-    <t>TOSHIBA</t>
-  </si>
-  <si>
-    <t>1225823</t>
-  </si>
-  <si>
-    <t>DIP8_VISHAY_6N13</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/808691.pdf</t>
-  </si>
-  <si>
-    <t>U59</t>
-  </si>
-  <si>
-    <t>16b I/O Expander</t>
-  </si>
-  <si>
-    <t>MCP23017-E/SO</t>
-  </si>
-  <si>
-    <t>1332087</t>
-  </si>
-  <si>
-    <t>SO14NB</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/12179.pdf</t>
-  </si>
-  <si>
-    <t>U61</t>
-  </si>
-  <si>
     <t>Quad DAC Package</t>
   </si>
   <si>
@@ -1548,7 +1598,7 @@
     <t>http://www.farnell.com/datasheets/74794.pdf</t>
   </si>
   <si>
-    <t>U62, U63</t>
+    <t>U58, U59</t>
   </si>
   <si>
     <t>Dual DigiPot non volatile 10Klog I2C</t>
@@ -1563,6 +1613,9 @@
     <t>2768195</t>
   </si>
   <si>
+    <t>http://www.farnell.com/datasheets/2313394.pdf</t>
+  </si>
+  <si>
     <t>VR1, VR2</t>
   </si>
   <si>
@@ -1612,6 +1665,9 @@
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/29611.pdf</t>
+  </si>
+  <si>
+    <t>WURTH ELEKTRONIK_693063020911</t>
   </si>
 </sst>
 </file>
@@ -1961,9 +2017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3107,150 +3165,150 @@
         <v>184</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="3">
-        <v>4</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="G34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="3">
-        <v>3</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>201</v>
+        <v>15</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>200</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="J35" s="2" t="s">
-        <v>125</v>
+        <v>202</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>17</v>
@@ -3259,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>125</v>
+        <v>214</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>125</v>
@@ -3291,36 +3349,36 @@
         <v>17</v>
       </c>
       <c r="H38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>17</v>
@@ -3329,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>125</v>
@@ -3340,22 +3398,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>17</v>
@@ -3364,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>125</v>
@@ -3375,22 +3433,22 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
@@ -3399,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>125</v>
@@ -3410,92 +3468,92 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>163</v>
+        <v>233</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>166</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H43" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>237</v>
+        <v>125</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>17</v>
@@ -3504,30 +3562,30 @@
         <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>247</v>
@@ -3536,7 +3594,7 @@
         <v>17</v>
       </c>
       <c r="H45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>248</v>
@@ -3556,13 +3614,13 @@
         <v>125</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>253</v>
@@ -3574,33 +3632,33 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>15</v>
+        <v>260</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>17</v>
@@ -3609,313 +3667,313 @@
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>263</v>
+        <v>125</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="H48" s="3">
-        <v>185</v>
+        <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>125</v>
+        <v>272</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>125</v>
+        <v>273</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="H49" s="3">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>125</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="H50" s="3">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="H51" s="3">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>283</v>
+        <v>125</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>284</v>
+        <v>125</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="H52" s="3">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>280</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="H53" s="3">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H54" s="3">
-        <v>53</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H55" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>17</v>
@@ -3924,453 +3982,453 @@
         <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>277</v>
+        <v>306</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>295</v>
+        <v>212</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H57" s="3">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>125</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H58" s="3">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>125</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="E59" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="G59" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H59" s="3">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H60" s="3">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>280</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H61" s="3">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H62" s="3">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H63" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H64" s="3">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H65" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>332</v>
+        <v>298</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H66" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H67" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>125</v>
+        <v>343</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>335</v>
+        <v>284</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>337</v>
+        <v>212</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H68" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>17</v>
@@ -4379,13 +4437,13 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -4402,10 +4460,10 @@
         <v>349</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>135</v>
+        <v>350</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>17</v>
@@ -4414,30 +4472,30 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>357</v>
@@ -4472,7 +4530,7 @@
         <v>362</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>356</v>
+        <v>135</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>363</v>
@@ -4513,10 +4571,10 @@
         <v>370</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>201</v>
+        <v>17</v>
       </c>
       <c r="H73" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>371</v>
@@ -4542,10 +4600,10 @@
         <v>375</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>17</v>
@@ -4554,36 +4612,36 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K74" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>383</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="H75" s="3">
         <v>1</v>
@@ -4647,10 +4705,10 @@
         <v>395</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>17</v>
@@ -4659,33 +4717,33 @@
         <v>1</v>
       </c>
       <c r="I77" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K77" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>17</v>
@@ -4694,33 +4752,33 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K78" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>17</v>
@@ -4729,33 +4787,33 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K79" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>418</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>17</v>
@@ -4764,68 +4822,68 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K80" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" s="3">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H81" s="3">
-        <v>4</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="J81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>125</v>
+        <v>426</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>17</v>
@@ -4834,173 +4892,173 @@
         <v>1</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>356</v>
+        <v>437</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H83" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>135</v>
+        <v>444</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H84" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>448</v>
+        <v>369</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H85" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>436</v>
+        <v>457</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H86" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>437</v>
+        <v>458</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>438</v>
+        <v>459</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>128</v>
+        <v>463</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>17</v>
@@ -5009,208 +5067,208 @@
         <v>3</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>440</v>
+        <v>468</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>356</v>
+        <v>135</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H88" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>467</v>
+        <v>128</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H89" s="3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>384</v>
+        <v>473</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>135</v>
+        <v>369</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H90" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>443</v>
+        <v>458</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>135</v>
+        <v>482</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H91" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>479</v>
+        <v>397</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H92" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>443</v>
+        <v>458</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>446</v>
+        <v>491</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>447</v>
+        <v>492</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>448</v>
+        <v>135</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>449</v>
+        <v>493</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>17</v>
@@ -5219,68 +5277,68 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>443</v>
+        <v>494</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>451</v>
+        <v>495</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>483</v>
+        <v>496</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>467</v>
+        <v>135</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H94" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>487</v>
+        <v>458</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>490</v>
+        <v>461</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>491</v>
+        <v>462</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>492</v>
+        <v>463</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>493</v>
+        <v>464</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>17</v>
@@ -5289,68 +5347,68 @@
         <v>1</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>494</v>
+        <v>458</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>495</v>
+        <v>466</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>417</v>
+        <v>482</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H96" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>17</v>
@@ -5359,153 +5417,223 @@
         <v>1</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>512</v>
+        <v>416</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H98" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>450</v>
+        <v>515</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>125</v>
+        <v>516</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>356</v>
+        <v>520</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H99" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H100" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>524</v>
+        <v>465</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>417</v>
+        <v>369</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H101" s="3">
+        <v>2</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102" s="3">
         <v>1</v>
       </c>
-      <c r="I101" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>530</v>
+      <c r="I102" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="3">
+        <v>1</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K103" s="2" t="s">
+        <v>546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new NAND option and fixe button footprint and re-add very complex double GND footprint
</commit_message>
<xml_diff>
--- a/Bill of Materials-Michel.xlsx
+++ b/Bill of Materials-Michel.xlsx
@@ -3,11 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocal\Desktop\electronic-levelup-hardware\Michel\Project Outputs for Michel\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24015" windowHeight="15825"/>
   </bookViews>
@@ -689,6 +684,9 @@
     <t>2081361</t>
   </si>
   <si>
+    <t>WURTH ELEKTRONIK_693063020911</t>
+  </si>
+  <si>
     <t>http://www.farnell.com/datasheets/1912447.pdf</t>
   </si>
   <si>
@@ -1157,7 +1155,7 @@
     <t>2494119</t>
   </si>
   <si>
-    <t>BGA324C80P18X18_800X1508X1508</t>
+    <t>ZCZ324</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/am3352.pdf</t>
@@ -1190,19 +1188,19 @@
     <t>Mémoire Flash/NAND</t>
   </si>
   <si>
-    <t>S34ML01G200BHI000</t>
-  </si>
-  <si>
-    <t>Cypress Semiconductor</t>
-  </si>
-  <si>
-    <t>2646449</t>
-  </si>
-  <si>
-    <t>BGA-63_VBM063</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2148647.pdf</t>
+    <t>S34MS02G100BHI000</t>
+  </si>
+  <si>
+    <t>CYPRESS SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>2772804</t>
+  </si>
+  <si>
+    <t>VBM063</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2330450.pdf</t>
   </si>
   <si>
     <t>U7</t>
@@ -1665,9 +1663,6 @@
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/29611.pdf</t>
-  </si>
-  <si>
-    <t>WURTH ELEKTRONIK_693063020911</t>
   </si>
 </sst>
 </file>
@@ -2019,9 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3352,33 +3345,33 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>547</v>
+        <v>221</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>17</v>
@@ -3387,7 +3380,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>125</v>
@@ -3398,22 +3391,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>17</v>
@@ -3422,7 +3415,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>125</v>
@@ -3433,22 +3426,22 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
@@ -3457,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>125</v>
@@ -3468,22 +3461,22 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>17</v>
@@ -3492,33 +3485,33 @@
         <v>2</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>17</v>
@@ -3527,33 +3520,33 @@
         <v>4</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>17</v>
@@ -3562,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>125</v>
@@ -3573,22 +3566,22 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>17</v>
@@ -3597,18 +3590,18 @@
         <v>2</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>125</v>
@@ -3617,13 +3610,13 @@
         <v>125</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>17</v>
@@ -3632,33 +3625,33 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>17</v>
@@ -3667,33 +3660,33 @@
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>17</v>
@@ -3702,33 +3695,33 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>17</v>
@@ -3737,33 +3730,33 @@
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>17</v>
@@ -3772,33 +3765,33 @@
         <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>125</v>
@@ -3807,24 +3800,24 @@
         <v>185</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>125</v>
@@ -3842,7 +3835,7 @@
         <v>42</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>19</v>
@@ -3853,22 +3846,22 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>125</v>
@@ -3877,33 +3870,33 @@
         <v>75</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>17</v>
@@ -3912,33 +3905,33 @@
         <v>1</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>17</v>
@@ -3947,33 +3940,33 @@
         <v>2</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>17</v>
@@ -3982,33 +3975,33 @@
         <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>17</v>
@@ -4017,33 +4010,33 @@
         <v>53</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>17</v>
@@ -4052,33 +4045,33 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>17</v>
@@ -4087,33 +4080,33 @@
         <v>1</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>17</v>
@@ -4122,7 +4115,7 @@
         <v>33</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>19</v>
@@ -4133,22 +4126,22 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>17</v>
@@ -4157,33 +4150,33 @@
         <v>38</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>17</v>
@@ -4192,33 +4185,33 @@
         <v>5</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>17</v>
@@ -4227,33 +4220,33 @@
         <v>2</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>17</v>
@@ -4262,33 +4255,33 @@
         <v>23</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>17</v>
@@ -4297,33 +4290,33 @@
         <v>8</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>17</v>
@@ -4332,33 +4325,33 @@
         <v>10</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>17</v>
@@ -4367,33 +4360,33 @@
         <v>4</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>17</v>
@@ -4402,33 +4395,33 @@
         <v>4</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>17</v>
@@ -4437,33 +4430,33 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>17</v>
@@ -4472,33 +4465,33 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>17</v>
@@ -4507,33 +4500,33 @@
         <v>3</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>17</v>
@@ -4542,33 +4535,33 @@
         <v>1</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>17</v>
@@ -4577,33 +4570,33 @@
         <v>3</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>17</v>
@@ -4612,33 +4605,33 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>207</v>
@@ -4647,33 +4640,33 @@
         <v>1</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>17</v>
@@ -4682,33 +4675,33 @@
         <v>1</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>17</v>
@@ -4717,33 +4710,33 @@
         <v>1</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>17</v>
@@ -4752,33 +4745,33 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>17</v>
@@ -4787,33 +4780,33 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>17</v>
@@ -4822,33 +4815,33 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>17</v>
@@ -4857,33 +4850,33 @@
         <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>17</v>
@@ -4892,33 +4885,33 @@
         <v>1</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>17</v>
@@ -4927,33 +4920,33 @@
         <v>4</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>17</v>
@@ -4962,33 +4955,33 @@
         <v>1</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>17</v>
@@ -4997,33 +4990,33 @@
         <v>7</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>17</v>
@@ -5032,33 +5025,33 @@
         <v>2</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>17</v>
@@ -5067,33 +5060,33 @@
         <v>3</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>17</v>
@@ -5102,33 +5095,33 @@
         <v>4</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>17</v>
@@ -5137,33 +5130,33 @@
         <v>3</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>17</v>
@@ -5172,33 +5165,33 @@
         <v>3</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>17</v>
@@ -5207,33 +5200,33 @@
         <v>12</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>17</v>
@@ -5242,33 +5235,33 @@
         <v>4</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>17</v>
@@ -5277,33 +5270,33 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>135</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>17</v>
@@ -5312,33 +5305,33 @@
         <v>3</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>17</v>
@@ -5347,33 +5340,33 @@
         <v>1</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>17</v>
@@ -5382,33 +5375,33 @@
         <v>4</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>17</v>
@@ -5417,33 +5410,33 @@
         <v>1</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>17</v>
@@ -5452,33 +5445,33 @@
         <v>1</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>17</v>
@@ -5487,33 +5480,33 @@
         <v>1</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>17</v>
@@ -5522,33 +5515,33 @@
         <v>2</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>17</v>
@@ -5557,33 +5550,33 @@
         <v>2</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>17</v>
@@ -5592,33 +5585,33 @@
         <v>1</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>17</v>
@@ -5627,13 +5620,13 @@
         <v>1</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync Output File ; reannote schematic, sync datasheet, fixe 1201328 permutation
</commit_message>
<xml_diff>
--- a/Bill of Materials-Michel.xlsx
+++ b/Bill of Materials-Michel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24015" windowHeight="15825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31140" windowHeight="15825"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Michel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="541">
   <si>
     <t>Designator</t>
   </si>
@@ -411,7 +411,7 @@
     <t>2453269</t>
   </si>
   <si>
-    <t>SOD323</t>
+    <t>SOD323-M</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2288055.pdf</t>
@@ -432,7 +432,7 @@
     <t>9778349</t>
   </si>
   <si>
-    <t>MF03A</t>
+    <t>MF03A-M</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/lm4041-n.pdf</t>
@@ -636,546 +636,531 @@
     <t>P1</t>
   </si>
   <si>
-    <t>Protoboard Olimex</t>
-  </si>
-  <si>
-    <t>AM3352-SOM-EVB</t>
+    <t>Connecteur USB-Type-B</t>
+  </si>
+  <si>
+    <t>1734346-1</t>
+  </si>
+  <si>
+    <t>TE CONNECTIVITY</t>
+  </si>
+  <si>
+    <t>1321918</t>
+  </si>
+  <si>
+    <t>CONN4_1-1734346</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/cad/1650080.pdf</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Embase mémoire</t>
+  </si>
+  <si>
+    <t>693063020911</t>
+  </si>
+  <si>
+    <t>WURTH ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>2081361</t>
+  </si>
+  <si>
+    <t>WURTH ELEKTRONIK_693063020911</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1912447.pdf</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Header, 3-Pin</t>
+  </si>
+  <si>
+    <t>1241150-3</t>
+  </si>
+  <si>
+    <t>9689478</t>
+  </si>
+  <si>
+    <t>CONN_1241150-3_T</t>
+  </si>
+  <si>
+    <t>P4, P6</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P7, P8</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>RK09K1130C79</t>
+  </si>
+  <si>
+    <t>ALPS</t>
+  </si>
+  <si>
+    <t>1191741</t>
+  </si>
+  <si>
+    <t>ALPS_RK09K1130C79</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2160634.pdf</t>
+  </si>
+  <si>
+    <t>P9, P10, P11, P12</t>
+  </si>
+  <si>
+    <t>P160KMP-0QC20B10K</t>
+  </si>
+  <si>
+    <t>Bi Technology</t>
+  </si>
+  <si>
+    <t>1760793</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2331843.pdf</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14, P15</t>
+  </si>
+  <si>
+    <t>DIN 5pin</t>
+  </si>
+  <si>
+    <t>PSG03463</t>
+  </si>
+  <si>
+    <t>PRO SIGNAL</t>
+  </si>
+  <si>
+    <t>1791756</t>
+  </si>
+  <si>
+    <t>PRO SIGNAL_PSG03463</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1697491.pdf</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>ABMM2-24.000MHZ-E2-T</t>
+  </si>
+  <si>
+    <t>ABRACON</t>
+  </si>
+  <si>
+    <t>2467855</t>
+  </si>
+  <si>
+    <t>SON440P360X120-4N</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1750519.pdf</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>32,768KHz</t>
+  </si>
+  <si>
+    <t>Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>LFXTAL003000</t>
+  </si>
+  <si>
+    <t>IQD FREQUENCY PRODUCTS</t>
+  </si>
+  <si>
+    <t>9713220</t>
+  </si>
+  <si>
+    <t>SON550P380X250-4N</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2175893.pdf</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>NPN Bipolar Transistor</t>
+  </si>
+  <si>
+    <t>SMMUN2214LT1G</t>
+  </si>
+  <si>
+    <t>9556672</t>
+  </si>
+  <si>
+    <t>SOT95P234X111-3N</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1813846.pdf</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>PNP Bipolar Transistor</t>
+  </si>
+  <si>
+    <t>SMMUN2114LT1G</t>
+  </si>
+  <si>
+    <t>2724481</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2237089.pdf</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>Ceramic Resonator</t>
+  </si>
+  <si>
+    <t>CSTCC8M00G53-R0</t>
+  </si>
+  <si>
+    <t>1170435</t>
+  </si>
+  <si>
+    <t>CSTCC_G</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/19296.pdf</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R97, R98, R99_Audio Input L, R99_Audio Input R, R99_Audio Repeat L, R99_Audio Repeat R, R100_Audio Input L, R100_Audio Input R, R100_Audio Repeat L, R100_Audio Repeat R, R101_Audio Input L, R101_Audio Input R, R101_Audio Repeat L, R101_Audio Repeat R, R102_Audio Input L, R102_Audio Input R, R102_Audio Repeat L, R102_Audio Repeat R, R103_Audio Input L, R103_Audio Input R, R103_Audio Repeat L, R103_Audio Repeat R, R104_Audio Input L, R104_Audio Input R, R104_Audio Repeat L, R104_Audio Repeat R, R105_Audio Output1, R105_Audio Output2, R105_Audio Output3, R106_Audio Output1, R106_Audio Output2, R106_Audio Output3, R107_Audio Output1, R107_Audio Output2, R107_Audio Output3, R108_Audio Output1, R108_Audio Output2, R108_Audio Output3, R109_Audio Output1, R109_Audio Output2, R109_Audio Output3, R110_Audio Output1, R110_Audio Output2, R110_Audio Output3, R111_Audio Output1, R111_Audio Output2, R111_Audio Output3, R112_Audio Output1, R112_Audio Output2, R112_Audio Output3, R113_Audio Output1, R113_Audio Output2, R113_Audio Output3, R114_Audio Output1, R114_Audio Output2, R114_Audio Output3, R115_Audio Output1, R115_Audio Output2, R115_Audio Output3, R116_Audio Output1, R116_Audio Output2, R116_Audio Output3, R117_Audio Output1, R117_Audio Output2, R117_Audio Output3, R118_Audio Output1, R118_Audio Output2, R118_Audio Output3, R296, R297, R298, R299, R300, R301, R302, R303, R305, R308, R311, R314</t>
+  </si>
+  <si>
+    <t>DNI, DNI, DNI, DNI, DNI, DNI, DNI, DNI, 10k, 10k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 1.5k, 1.5k, 1.5k, 1.5k, 3k, 3k, 3k, 3k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 10k, 20k, 10k, 20k, 10k, 20k, 10k, 20k, 0, 0, 0, 0</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2483933, 2483933, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2613050, 2613050, 2613050, 2613050, 2331191, 2331191, 2331191, 2331191, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029, [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>RESC1608X05</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, [NoParam], [NoParam], [NoParam], [NoParam]</t>
+  </si>
+  <si>
+    <t>R9, R10, R11, R12, R131, R132, R133, R162_MS - LR Converter1, R162_MS - LR Converter2, R163_MS - LR Converter1, R163_MS - LR Converter2, R164, R168, R192, R193, R194, R235, R236, R237, R259_Mode Select 1A, R259_Mode Select 1B, R259_Mode Select 2A, R259_Mode Select 2B, R260_Mode Select 1A, R260_Mode Select 1B, R260_Mode Select 2A, R260_Mode Select 2B, R261_Mode Select 1A, R261_Mode Select 1B, R261_Mode Select 2A, R261_Mode Select 2B, R262, R263, R273, R274, R275, R290, R291, R292, R293, R294, R295</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>R13, R14, R15, R16, R17, R18, R19, R20, R21, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R73, R74, R75, R76, R77, R78, R79, R80, R81, R82, R83, R84, R85, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96</t>
+  </si>
+  <si>
+    <t>0, 0, 10k, 10k, 100k, 100k, 0, 0, 10k, 1.2k, 0, DNI, 10k, DNI, DNI, 100K, DNI, DNI, DNI, DNI, DNI, DNI, 100K, DNI, DNI, DNI, DNI, 100K, DNI, 100K, 100K, DNI, 100K, 100K, 100K, 100K, 100K, 100K, DNI, 100K, 100K, 100K, 100K, DNI, 100K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B1K2E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], 2483933, 2483933, 2687850, 2687850, [NoParam], [NoParam], 2483933, 2483896, [NoParam], [NoParam], 2483933, [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021</t>
+  </si>
+  <si>
+    <t>[NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B4K7E1</t>
+  </si>
+  <si>
+    <t>2483933</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1935020.pdf</t>
+  </si>
+  <si>
+    <t>R23, R24</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B1K0E1</t>
+  </si>
+  <si>
+    <t>2483880</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26, R27, R29, R119, R120, R121, R123, R125, R127, R128, R130, R134, R135, R136, R138, R140, R142, R143, R145, R146_MS - LR Converter1, R146_MS - LR Converter2, R147_MS - LR Converter1, R147_MS - LR Converter2, R148_MS - LR Converter1, R148_MS - LR Converter2, R149_MS - LR Converter1, R149_MS - LR Converter2, R150_MS - LR Converter1, R150_MS - LR Converter2, R151_MS - LR Converter1, R151_MS - LR Converter2, R153_MS - LR Converter1, R153_MS - LR Converter2, R154_MS - LR Converter1, R154_MS - LR Converter2, R155_MS - LR Converter1, R155_MS - LR Converter2, R156_MS - LR Converter1, R156_MS - LR Converter2, R157_MS - LR Converter1, R157_MS - LR Converter2, R158_MS - LR Converter1, R158_MS - LR Converter2, R159_MS - LR Converter1, R159_MS - LR Converter2, R160_MS - LR Converter1, R160_MS - LR Converter2, R166, R170, R268, R269, R280, R281</t>
+  </si>
+  <si>
+    <t>1K, 1K, 1K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B1K0E1, CPF-A-0603B1K0E1, CPF-A-0603B1K0E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1</t>
+  </si>
+  <si>
+    <t>2483880, 2483880, 2483880, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R72, R175, R176, R177, R178, R179, R180, R183, R188, R198, R199, R200, R201, R202, R203, R206, R211, R218, R219, R220, R221, R222, R223, R226, R231, R241, R242, R243, R244, R245, R246, R249, R254</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B33KE1</t>
+  </si>
+  <si>
+    <t>2483920</t>
+  </si>
+  <si>
+    <t>R122, R124, R129, R137, R139, R144, R152_MS - LR Converter1, R152_MS - LR Converter2, R161_MS - LR Converter1, R161_MS - LR Converter2, R165, R169, R172, R173, R174, R189, R191, R195, R196, R197, R212, R214, R215, R216, R217, R232, R234, R238, R239, R240, R255, R257, R266, R267, R272, R278, R279, R284</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>RN73C1J100KBTDF</t>
+  </si>
+  <si>
+    <t>2687850</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2189072.pdf</t>
+  </si>
+  <si>
+    <t>R126, R141, R285, R288, R289</t>
+  </si>
+  <si>
+    <t>220k</t>
+  </si>
+  <si>
+    <t>CPF-A-0603B220KE1</t>
+  </si>
+  <si>
+    <t>2483903</t>
+  </si>
+  <si>
+    <t>R167, R171</t>
+  </si>
+  <si>
+    <t>13k</t>
+  </si>
+  <si>
+    <t>CPF0603B13KE1</t>
+  </si>
+  <si>
+    <t>2330920</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2104089.pdf</t>
+  </si>
+  <si>
+    <t>R181, R182, R190, R204, R205, R213, R224, R225, R233, R247, R248, R256, R264, R276, R287, R304, R306, R307, R309, R310, R312, R313, R315</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R184, R185, R207, R208, R227, R228, R250, R251</t>
+  </si>
+  <si>
+    <t>51k</t>
+  </si>
+  <si>
+    <t>CPF0603B51KE1</t>
+  </si>
+  <si>
+    <t>2331265</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2043335.pdf</t>
+  </si>
+  <si>
+    <t>R186, R187, R209, R210, R229, R230, R252, R253, R271, R283</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>R258_Mode Select 1A, R258_Mode Select 1B, R258_Mode Select 2A, R258_Mode Select 2B</t>
+  </si>
+  <si>
+    <t>470k</t>
+  </si>
+  <si>
+    <t>CPF0603B470KE1</t>
+  </si>
+  <si>
+    <t>2331232</t>
+  </si>
+  <si>
+    <t>R265, R270, R277, R282</t>
+  </si>
+  <si>
+    <t>150k</t>
+  </si>
+  <si>
+    <t>CPF0603B150KE1</t>
+  </si>
+  <si>
+    <t>2330937</t>
+  </si>
+  <si>
+    <t>R286</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SPDT Subminiature Toggle Switch, Right Angle Mounting, Vertical Actuation</t>
+  </si>
+  <si>
+    <t>TS01ABE</t>
+  </si>
+  <si>
+    <t>C &amp; K COMPONENTS</t>
+  </si>
+  <si>
+    <t>2435185</t>
+  </si>
+  <si>
+    <t>C&amp;K_TS01ABE</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1839865.pdf</t>
+  </si>
+  <si>
+    <t>S2, S3, S4</t>
+  </si>
+  <si>
+    <t>Commutateur tactile</t>
+  </si>
+  <si>
+    <t>KMR211G LFS</t>
+  </si>
+  <si>
+    <t>1437635</t>
+  </si>
+  <si>
+    <t>C&amp;K_KMR211G</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/2044619.pdf</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Gestion d'alimentation PMIC</t>
+  </si>
+  <si>
+    <t>TPS65217CRSLT</t>
+  </si>
+  <si>
+    <t>2492485</t>
+  </si>
+  <si>
+    <t>CRSLT</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tps65217.pdf</t>
+  </si>
+  <si>
+    <t>U2, U6, U54</t>
+  </si>
+  <si>
+    <t>Buffers &amp; Transmetteurs</t>
+  </si>
+  <si>
+    <t>SN74LVC1G07DCKR</t>
+  </si>
+  <si>
+    <t>Texas Instrument</t>
+  </si>
+  <si>
+    <t>1287544</t>
+  </si>
+  <si>
+    <t>DCK5</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn74lvc1g07.pdf</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Microprocesseur ARM</t>
+  </si>
+  <si>
+    <t>AM3352BZCZ100</t>
+  </si>
+  <si>
+    <t>2494119</t>
+  </si>
+  <si>
+    <t>ZCZ324</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/am3352.pdf</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Mémoire DDR3/SRAM</t>
+  </si>
+  <si>
+    <t>DS_K4B4G1646D</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>K4B4G1646D-BCK0</t>
   </si>
   <si>
     <t>Olimex</t>
   </si>
   <si>
-    <t>https://www.olimex.com/Products/SOM/AM335X/AM3352-SOM/resources/AM3352-SOM-UM.pdf</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>Connecteur USB-Type-B</t>
-  </si>
-  <si>
-    <t>1734346-1</t>
-  </si>
-  <si>
-    <t>TE CONNECTIVITY</t>
-  </si>
-  <si>
-    <t>1321918</t>
-  </si>
-  <si>
-    <t>CONN4_1-1734346</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/cad/1650080.pdf</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Embase mémoire</t>
-  </si>
-  <si>
-    <t>693063020911</t>
-  </si>
-  <si>
-    <t>WURTH ELEKTRONIK</t>
-  </si>
-  <si>
-    <t>2081361</t>
-  </si>
-  <si>
-    <t>WURTH ELEKTRONIK_693063020911</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1912447.pdf</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>Header, 3-Pin</t>
-  </si>
-  <si>
-    <t>1241150-3</t>
-  </si>
-  <si>
-    <t>2399724</t>
-  </si>
-  <si>
-    <t>CONN_1241150-3_T</t>
-  </si>
-  <si>
-    <t>P5, P7</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P8, P9</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>RK09K1130C79</t>
-  </si>
-  <si>
-    <t>ALPS</t>
-  </si>
-  <si>
-    <t>1191741</t>
-  </si>
-  <si>
-    <t>ALPS_RK09K1130C79</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2160634.pdf</t>
-  </si>
-  <si>
-    <t>P10, P11, P12, P13</t>
-  </si>
-  <si>
-    <t>P160KMP-0QC20B10K</t>
-  </si>
-  <si>
-    <t>Bi Technology</t>
-  </si>
-  <si>
-    <t>1760793</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2331843.pdf</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P15, P16</t>
-  </si>
-  <si>
-    <t>DIN 5pin</t>
-  </si>
-  <si>
-    <t>PSG03463</t>
-  </si>
-  <si>
-    <t>PRO SIGNAL</t>
-  </si>
-  <si>
-    <t>1791756</t>
-  </si>
-  <si>
-    <t>PRO SIGNAL_PSG03463</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1697491.pdf</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>ABMM2-24.000MHZ-E2-T</t>
-  </si>
-  <si>
-    <t>ABRACON</t>
-  </si>
-  <si>
-    <t>2467855</t>
-  </si>
-  <si>
-    <t>SON440P360X120-4N</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1750519.pdf</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>32,768KHz</t>
-  </si>
-  <si>
-    <t>Crystal Oscillator</t>
-  </si>
-  <si>
-    <t>LFXTAL003000</t>
-  </si>
-  <si>
-    <t>IQD FREQUENCY PRODUCTS</t>
-  </si>
-  <si>
-    <t>9713220</t>
-  </si>
-  <si>
-    <t>SON550P380X250-4N</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2175893.pdf</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>NPN Bipolar Transistor</t>
-  </si>
-  <si>
-    <t>SMMUN2214LT1G</t>
-  </si>
-  <si>
-    <t>9556672</t>
-  </si>
-  <si>
-    <t>SOT95P234X111-3N</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1813846.pdf</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>PNP Bipolar Transistor</t>
-  </si>
-  <si>
-    <t>SMMUN2114LT1G</t>
-  </si>
-  <si>
-    <t>2724481</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2237089.pdf</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>8MHz</t>
-  </si>
-  <si>
-    <t>Ceramic Resonator</t>
-  </si>
-  <si>
-    <t>CSTCC8M00G53-R0</t>
-  </si>
-  <si>
-    <t>1170435</t>
-  </si>
-  <si>
-    <t>CSTCC_G</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/19296.pdf</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R72, R73, R74, R75, R76, R77, R78, R79, R80, R81, R103, R104, R105, R106, R107, R108, R109, R110, R111, R112, R113, R114, R115, R116, R117, R118, R119, R120, R121, R122, R123, R124, R125, R126, R195, R196, R197_Audio Input L, R197_Audio Input R, R197_Audio Repeat L, R197_Audio Repeat R, R198_Audio Input L, R198_Audio Input R, R198_Audio Repeat L, R198_Audio Repeat R, R199_Audio Input L, R199_Audio Input R, R199_Audio Repeat L, R199_Audio Repeat R, R200_Audio Input L, R200_Audio Input R, R200_Audio Repeat L, R200_Audio Repeat R, R201_Audio Input L, R201_Audio Input R, R201_Audio Repeat L, R201_Audio Repeat R, R202_Audio Input L, R202_Audio Input R, R202_Audio Repeat L, R202_Audio Repeat R, R203_Audio Output1, R203_Audio Output2, R203_Audio Output3, R204_Audio Output1, R204_Audio Output2, R204_Audio Output3, R205_Audio Output1, R205_Audio Output2, R205_Audio Output3, R206_Audio Output1, R206_Audio Output2, R206_Audio Output3, R207_Audio Output1, R207_Audio Output2, R207_Audio Output3, R208_Audio Output1, R208_Audio Output2, R208_Audio Output3, R209_Audio Output1, R209_Audio Output2, R209_Audio Output3, R210_Audio Output1, R210_Audio Output2, R210_Audio Output3, R211_Audio Output1, R211_Audio Output2, R211_Audio Output3, R212_Audio Output1, R212_Audio Output2, R212_Audio Output3, R213_Audio Output1, R213_Audio Output2, R213_Audio Output3, R214_Audio Output1, R214_Audio Output2, R214_Audio Output3, R215_Audio Output1, R215_Audio Output2, R215_Audio Output3, R216_Audio Output1, R216_Audio Output2, R216_Audio Output3, R394, R395, R396, R397, R398, R399, R400, R401, R403, R406, R409, R412</t>
-  </si>
-  <si>
-    <t>0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, DNI, 0, 0, DNI, 0, 0, 0, 0, 0, 0, 0, 0, DNI, 0, 0, DNI, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, DNI, DNI, DNI, DNI, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 10k, 10k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 1.5k, 1.5k, 1.5k, 1.5k, 3k, 3k, 3k, 3k, 1.5k, 1.5k, 1.5k, 1.5k, 47Ohm, 47Ohm, 47Ohm, 47Ohm, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 11k, 11k, 11k, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 47Ohm, 47Ohm, 47Ohm, 15k, 15k, 15k, 820Ohm, 820Ohm, 820Ohm, 11k, 11k, 11k, 10k, 20k, 10k, 20k, 10k, 20k, 10k, 20k, 0, 0, 0, 0</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, CPF0603B3K0E1, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, RN73C1J1K5BTDF, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF-A-0603B47RE1, CPF0603B15KE1, CPF0603B15KE1, CPF0603B15KE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF-A-0603B820RE1, CPF0603B11KE1, CPF0603B11KE1, CPF0603B11KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, CPF-A-0603B4K7E1, CPF0603B20KE1, [NoParam], [NoParam], [NoParam], [NoParam]</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2483933, 2483933, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2613050, 2613050, 2613050, 2613050, 2331191, 2331191, 2331191, 2331191, 2613050, 2613050, 2613050, 2613050, 2483931, 2483931, 2483931, 2483931, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2330892, 2330892, 2330892, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2483931, 2483931, 2483931, 2615493, 2615493, 2615493, 2483946, 2483946, 2483946, 2330892, 2330892, 2330892, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029, 2483933, 2331029, [NoParam], [NoParam], [NoParam], [NoParam]</t>
-  </si>
-  <si>
-    <t>RESC1608X05</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2043336.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/2170353.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/2104089.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2170367.pdf, [NoParam], [NoParam], [NoParam], [NoParam]</t>
-  </si>
-  <si>
-    <t>R82, R83, R84, R85, R229, R230, R231, R260_MS - LR Converter1, R260_MS - LR Converter2, R261_MS - LR Converter1, R261_MS - LR Converter2, R262, R266, R290, R291, R292, R333, R334, R335, R357_Mode Select 1A, R357_Mode Select 1B, R357_Mode Select 2A, R357_Mode Select 2B, R358_Mode Select 1A, R358_Mode Select 1B, R358_Mode Select 2A, R358_Mode Select 2B, R359_Mode Select 1A, R359_Mode Select 1B, R359_Mode Select 2A, R359_Mode Select 2B, R360, R361, R371, R372, R373, R388, R389, R390, R391, R392, R393</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>R86, R87, R88, R89, R90, R91, R92, R93, R94, R128, R129, R130, R131, R132, R133, R134, R135, R136, R137, R138, R139, R140, R141, R142, R143, R144, R145, R146, R147, R148, R149, R150, R151, R152, R153, R154, R155, R156, R157, R158, R159, R160, R161, R162, R163, R164, R165, R166, R167, R168, R169, R171, R172, R173, R174, R175, R176, R177, R178, R179, R180, R181, R182, R183, R184, R185, R186, R187, R188, R189, R190, R191, R192, R193, R194</t>
-  </si>
-  <si>
-    <t>0, 0, 10k, 10k, 100k, 100k, 0, 0, 10k, 1.2k, 0, DNI, 10k, DNI, DNI, 100K, DNI, DNI, DNI, DNI, DNI, DNI, 100K, DNI, DNI, DNI, DNI, 100K, DNI, 100K, 100K, DNI, 100K, 100K, 100K, 100K, 100K, 100K, DNI, 100K, 100K, 100K, 100K, DNI, 100K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k, 10k, 27k</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], [NoParam], CPF-A-0603B4K7E1, CPF-A-0603B1K2E1, [NoParam], [NoParam], CPF-A-0603B4K7E1, [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], [NoParam], [NoParam], [NoParam], RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, RN73C1J100KBTDF, [NoParam], RN73C1J100KBTDF, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K, CPF-A-0603B4K7E1, CRGH0603F27K</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], 2483933, 2483933, 2687850, 2687850, [NoParam], [NoParam], 2483933, 2483896, [NoParam], [NoParam], 2483933, [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], [NoParam], [NoParam], [NoParam], 2687850, [NoParam], 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2687850, 2687850, 2687850, [NoParam], 2687850, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021, 2483933, 2332021</t>
-  </si>
-  <si>
-    <t>[NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/1935020.pdf, [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], [NoParam], [NoParam], [NoParam], http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/2189072.pdf, [NoParam], http://www.farnell.com/datasheets/2189072.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf, http://www.farnell.com/datasheets/1935020.pdf, http://www.farnell.com/datasheets/1755795.pdf</t>
-  </si>
-  <si>
-    <t>R95</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B4K7E1</t>
-  </si>
-  <si>
-    <t>2483933</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1935020.pdf</t>
-  </si>
-  <si>
-    <t>R96, R97</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B1K0E1</t>
-  </si>
-  <si>
-    <t>2483880</t>
-  </si>
-  <si>
-    <t>R98</t>
-  </si>
-  <si>
-    <t>R99, R100, R127, R217, R218, R219, R221, R223, R225, R226, R228, R232, R233, R234, R236, R238, R240, R241, R243, R244_MS - LR Converter1, R244_MS - LR Converter2, R245_MS - LR Converter1, R245_MS - LR Converter2, R246_MS - LR Converter1, R246_MS - LR Converter2, R247_MS - LR Converter1, R247_MS - LR Converter2, R248_MS - LR Converter1, R248_MS - LR Converter2, R249_MS - LR Converter1, R249_MS - LR Converter2, R251_MS - LR Converter1, R251_MS - LR Converter2, R252_MS - LR Converter1, R252_MS - LR Converter2, R253_MS - LR Converter1, R253_MS - LR Converter2, R254_MS - LR Converter1, R254_MS - LR Converter2, R255_MS - LR Converter1, R255_MS - LR Converter2, R256_MS - LR Converter1, R256_MS - LR Converter2, R257_MS - LR Converter1, R257_MS - LR Converter2, R258_MS - LR Converter1, R258_MS - LR Converter2, R264, R268, R366, R367, R378, R379</t>
-  </si>
-  <si>
-    <t>1K, 1K, 1K, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k, 10k</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B1K0E1, CPF-A-0603B1K0E1, CPF-A-0603B1K0E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1, CPF-A-0603B4K7E1</t>
-  </si>
-  <si>
-    <t>2483880, 2483880, 2483880, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933, 2483933</t>
-  </si>
-  <si>
-    <t>R101</t>
-  </si>
-  <si>
-    <t>R102</t>
-  </si>
-  <si>
-    <t>R170, R273, R274, R275, R276, R277, R278, R281, R286, R296, R297, R298, R299, R300, R301, R304, R309, R316, R317, R318, R319, R320, R321, R324, R329, R339, R340, R341, R342, R343, R344, R347, R352</t>
-  </si>
-  <si>
-    <t>33k</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B33KE1</t>
-  </si>
-  <si>
-    <t>2483920</t>
-  </si>
-  <si>
-    <t>R220, R222, R227, R235, R237, R242, R250_MS - LR Converter1, R250_MS - LR Converter2, R259_MS - LR Converter1, R259_MS - LR Converter2, R263, R267, R270, R271, R272, R287, R289, R293, R294, R295, R310, R312, R313, R314, R315, R330, R332, R336, R337, R338, R353, R355, R364, R365, R370, R376, R377, R382</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>RN73C1J100KBTDF</t>
-  </si>
-  <si>
-    <t>2687850</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2189072.pdf</t>
-  </si>
-  <si>
-    <t>R224, R239, R383, R386, R387</t>
-  </si>
-  <si>
-    <t>220k</t>
-  </si>
-  <si>
-    <t>CPF-A-0603B220KE1</t>
-  </si>
-  <si>
-    <t>2483903</t>
-  </si>
-  <si>
-    <t>R265, R269</t>
-  </si>
-  <si>
-    <t>13k</t>
-  </si>
-  <si>
-    <t>CPF0603B13KE1</t>
-  </si>
-  <si>
-    <t>2330920</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2104089.pdf</t>
-  </si>
-  <si>
-    <t>R279, R280, R288, R302, R303, R311, R322, R323, R331, R345, R346, R354, R362, R374, R385, R402, R404, R405, R407, R408, R410, R411, R413</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R282, R283, R305, R306, R325, R326, R348, R349</t>
-  </si>
-  <si>
-    <t>51k</t>
-  </si>
-  <si>
-    <t>CPF0603B51KE1</t>
-  </si>
-  <si>
-    <t>2331265</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2043335.pdf</t>
-  </si>
-  <si>
-    <t>R284, R285, R307, R308, R327, R328, R350, R351, R369, R381</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>R356_Mode Select 1A, R356_Mode Select 1B, R356_Mode Select 2A, R356_Mode Select 2B</t>
-  </si>
-  <si>
-    <t>470k</t>
-  </si>
-  <si>
-    <t>CPF0603B470KE1</t>
-  </si>
-  <si>
-    <t>2331232</t>
-  </si>
-  <si>
-    <t>R363, R368, R375, R380</t>
-  </si>
-  <si>
-    <t>150k</t>
-  </si>
-  <si>
-    <t>CPF0603B150KE1</t>
-  </si>
-  <si>
-    <t>2330937</t>
-  </si>
-  <si>
-    <t>R384</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>SPDT Subminiature Toggle Switch, Right Angle Mounting, Vertical Actuation</t>
-  </si>
-  <si>
-    <t>TS01ABE</t>
-  </si>
-  <si>
-    <t>C &amp; K COMPONENTS</t>
-  </si>
-  <si>
-    <t>2435185</t>
-  </si>
-  <si>
-    <t>C&amp;K_TS01ABE</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1839865.pdf</t>
-  </si>
-  <si>
-    <t>S2, S3, S4</t>
-  </si>
-  <si>
-    <t>Commutateur tactile</t>
-  </si>
-  <si>
-    <t>KMR211G LFS</t>
-  </si>
-  <si>
-    <t>1437635</t>
-  </si>
-  <si>
-    <t>C&amp;K_KMR211G</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2044619.pdf</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Gestion d'alimentation PMIC</t>
-  </si>
-  <si>
-    <t>TPS65217CRSLT</t>
-  </si>
-  <si>
-    <t>2492485</t>
-  </si>
-  <si>
-    <t>CRSLT</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tps65217.pdf</t>
-  </si>
-  <si>
-    <t>U2, U6, U54</t>
-  </si>
-  <si>
-    <t>Buffers &amp; Transmetteurs</t>
-  </si>
-  <si>
-    <t>SN74LVC1G07DCKR</t>
-  </si>
-  <si>
-    <t>Texas Instrument</t>
-  </si>
-  <si>
-    <t>1287544</t>
-  </si>
-  <si>
-    <t>DCK5</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/sn74lvc1g07.pdf</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>Microprocesseur ARM</t>
-  </si>
-  <si>
-    <t>AM3352BZCZ100</t>
-  </si>
-  <si>
-    <t>2494119</t>
-  </si>
-  <si>
-    <t>ZCZ324</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/am3352.pdf</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>Mémoire DDR3/SRAM</t>
-  </si>
-  <si>
-    <t>DS_K4B4G1646D</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>K4B4G1646D-BCK0</t>
-  </si>
-  <si>
     <t>BGA96C80P16X6_133X75X11</t>
   </si>
   <si>
@@ -1215,7 +1200,7 @@
     <t>2335452</t>
   </si>
   <si>
-    <t>DBV6</t>
+    <t>DBV6-M</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/tpd4e001.pdf</t>
@@ -1278,7 +1263,7 @@
     <t>1292241</t>
   </si>
   <si>
-    <t>PDIP16_300MC</t>
+    <t>SOIC16_MCP3008</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/808965.pdf</t>
@@ -1299,7 +1284,7 @@
     <t>1972086</t>
   </si>
   <si>
-    <t>32A</t>
+    <t>32A-M</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2047852.pdf</t>
@@ -1320,7 +1305,7 @@
     <t>2519520</t>
   </si>
   <si>
-    <t>21-0042B_24</t>
+    <t>21-0042B_24-M</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/1825883.pdf</t>
@@ -1362,7 +1347,7 @@
     <t>2496455</t>
   </si>
   <si>
-    <t>PAP64_7X7P26</t>
+    <t>PAP64_7X7P26-M</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/pcm3168a.pdf</t>
@@ -1380,7 +1365,7 @@
     <t>1103060</t>
   </si>
   <si>
-    <t>D8</t>
+    <t>D8-M</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/ne5532a.pdf</t>
@@ -1392,19 +1377,19 @@
     <t>Quad Audio OpAmp</t>
   </si>
   <si>
-    <t>OPA1654AID</t>
+    <t>OPA1654</t>
   </si>
   <si>
     <t>2099889</t>
   </si>
   <si>
-    <t>D14</t>
+    <t>D14-M</t>
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/opa1654.pdf</t>
   </si>
   <si>
-    <t>U21, U31, U51</t>
+    <t>U21, U31, U36, U51</t>
   </si>
   <si>
     <t>Dual DigiPot non volatile I2C</t>
@@ -1413,13 +1398,10 @@
     <t>MCP4661-503E/ST</t>
   </si>
   <si>
-    <t>Microchip</t>
-  </si>
-  <si>
     <t>1840724</t>
   </si>
   <si>
-    <t>TSSOP14_MC</t>
+    <t>TSSOP14_MC-M</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/2243913.pdf</t>
@@ -1431,7 +1413,10 @@
     <t>Dual Audio OpAmp</t>
   </si>
   <si>
-    <t>U23_MS - LR Converter1, U23_MS - LR Converter2, U42</t>
+    <t>NE5532</t>
+  </si>
+  <si>
+    <t>U23_MS - LR Converter1, U23_MS - LR Converter2, U43</t>
   </si>
   <si>
     <t>Quad 2:1 Multiplexer</t>
@@ -1461,7 +1446,7 @@
     <t>http://www.ti.com/lit/ds/symlink/tl084.pdf</t>
   </si>
   <si>
-    <t>U26, U28, U40, U41, U43, U44, U45, U46, U47, U48, U49, U50</t>
+    <t>U26, U28, U40, U41, U42, U44, U45, U46, U47, U48, U49, U50</t>
   </si>
   <si>
     <t>Single 2:1 Multiplexer</t>
@@ -1494,7 +1479,7 @@
     <t>http://www.ti.com/lit/ds/symlink/cd4069ub.pdf</t>
   </si>
   <si>
-    <t>U30</t>
+    <t>U30, U33, U35, U38</t>
   </si>
   <si>
     <t>Dual Transconductance OpAmp</t>
@@ -1512,12 +1497,6 @@
     <t>http://www.ti.com/lit/ds/symlink/lm13700.pdf</t>
   </si>
   <si>
-    <t>U33, U35, U38</t>
-  </si>
-  <si>
-    <t>U36</t>
-  </si>
-  <si>
     <t>U39_Mode Select 1A, U39_Mode Select 1B, U39_Mode Select 2A, U39_Mode Select 2B</t>
   </si>
   <si>
@@ -1542,19 +1521,19 @@
     <t>Optocoupler</t>
   </si>
   <si>
-    <t>6N139</t>
-  </si>
-  <si>
-    <t>TOSHIBA</t>
-  </si>
-  <si>
-    <t>1225823</t>
+    <t>6N139-300E</t>
+  </si>
+  <si>
+    <t>BOADCOM</t>
+  </si>
+  <si>
+    <t>1085023</t>
   </si>
   <si>
     <t>DIP8_VISHAY_6N13</t>
   </si>
   <si>
-    <t>http://www.farnell.com/datasheets/808691.pdf</t>
+    <t>http://www.farnell.com/datasheets/1266261.pdf</t>
   </si>
   <si>
     <t>U55</t>
@@ -1569,7 +1548,7 @@
     <t>1332087</t>
   </si>
   <si>
-    <t>SO14NB</t>
+    <t>SOIC28_MCP23017</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/12179.pdf</t>
@@ -1590,7 +1569,7 @@
     <t>2518696</t>
   </si>
   <si>
-    <t>21-0061L</t>
+    <t>21-0061L-M</t>
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/74794.pdf</t>
@@ -2012,7 +1991,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3266,42 +3245,42 @@
         <v>207</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>17</v>
@@ -3310,33 +3289,33 @@
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>17</v>
@@ -3345,13 +3324,13 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3362,25 +3341,25 @@
         <v>125</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>125</v>
@@ -3391,31 +3370,31 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>163</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>125</v>
@@ -3426,66 +3405,66 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="F41" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H41" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>166</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>236</v>
+        <v>125</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>125</v>
@@ -3499,124 +3478,124 @@
         <v>238</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>231</v>
+        <v>125</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H43" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="G44" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>166</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>245</v>
+        <v>125</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>125</v>
+        <v>253</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>17</v>
@@ -3625,33 +3604,33 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>258</v>
+        <v>125</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>261</v>
+        <v>128</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>17</v>
@@ -3660,33 +3639,33 @@
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>17</v>
@@ -3695,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>125</v>
@@ -3709,19 +3688,19 @@
         <v>271</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>125</v>
+        <v>272</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>17</v>
@@ -3730,118 +3709,118 @@
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="H50" s="3">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H51" s="3">
+        <v>42</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H51" s="3">
-        <v>185</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>289</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="G52" s="2" t="s">
         <v>125</v>
       </c>
       <c r="H52" s="3">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3849,51 +3828,51 @@
         <v>292</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="G53" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="H53" s="3">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>298</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>299</v>
@@ -3902,68 +3881,68 @@
         <v>17</v>
       </c>
       <c r="H54" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H55" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>302</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>303</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>304</v>
@@ -3972,331 +3951,331 @@
         <v>17</v>
       </c>
       <c r="H56" s="3">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H57" s="3">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H58" s="3">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>300</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H59" s="3">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H60" s="3">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>125</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H61" s="3">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H62" s="3">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H63" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H64" s="3">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H65" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -4307,83 +4286,83 @@
         <v>338</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>299</v>
+        <v>340</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H66" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H67" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>346</v>
@@ -4392,71 +4371,71 @@
         <v>17</v>
       </c>
       <c r="H68" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>288</v>
+        <v>347</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>340</v>
+        <v>125</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>285</v>
+        <v>350</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>212</v>
+        <v>345</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H69" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>288</v>
+        <v>353</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>336</v>
+        <v>354</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>351</v>
+        <v>135</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>17</v>
@@ -4465,33 +4444,33 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>17</v>
@@ -4500,33 +4479,33 @@
         <v>3</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>135</v>
+        <v>364</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>17</v>
@@ -4535,68 +4514,68 @@
         <v>1</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>17</v>
+        <v>379</v>
       </c>
       <c r="H73" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>17</v>
@@ -4605,68 +4584,68 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="H75" s="3">
         <v>1</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>17</v>
@@ -4675,33 +4654,33 @@
         <v>1</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>370</v>
+        <v>405</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>17</v>
@@ -4710,33 +4689,33 @@
         <v>1</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>17</v>
@@ -4745,33 +4724,33 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>17</v>
@@ -4780,33 +4759,33 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>17</v>
@@ -4815,68 +4794,68 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H81" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>17</v>
@@ -4885,173 +4864,173 @@
         <v>1</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H83" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H84" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>370</v>
+        <v>412</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H85" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>135</v>
+        <v>440</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H86" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>464</v>
+        <v>128</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>17</v>
@@ -5060,173 +5039,173 @@
         <v>3</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>451</v>
+        <v>472</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>135</v>
+        <v>440</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>452</v>
+        <v>473</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H88" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>454</v>
+        <v>474</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>128</v>
+        <v>478</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H89" s="3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>474</v>
+        <v>393</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>456</v>
+        <v>482</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>370</v>
+        <v>440</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H90" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H91" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>398</v>
+        <v>490</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>135</v>
+        <v>478</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>17</v>
@@ -5235,33 +5214,33 @@
         <v>4</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>459</v>
+        <v>496</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>135</v>
+        <v>501</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>17</v>
@@ -5270,68 +5249,68 @@
         <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>135</v>
+        <v>412</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H94" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>459</v>
+        <v>509</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>498</v>
+        <v>511</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>462</v>
+        <v>512</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>463</v>
+        <v>513</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>464</v>
+        <v>514</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>465</v>
+        <v>515</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>17</v>
@@ -5340,103 +5319,103 @@
         <v>1</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>459</v>
+        <v>516</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>467</v>
+        <v>517</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>499</v>
+        <v>518</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>500</v>
+        <v>519</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>483</v>
+        <v>521</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>502</v>
+        <v>522</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H96" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>503</v>
+        <v>460</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>504</v>
+        <v>523</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>505</v>
+        <v>524</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>506</v>
+        <v>525</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>507</v>
+        <v>526</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>508</v>
+        <v>364</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H97" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>510</v>
+        <v>528</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>417</v>
+        <v>532</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>17</v>
@@ -5445,33 +5424,33 @@
         <v>1</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>516</v>
+        <v>534</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>520</v>
+        <v>537</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>521</v>
+        <v>412</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>17</v>
@@ -5480,153 +5459,13 @@
         <v>1</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H100" s="3">
-        <v>2</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H101" s="3">
-        <v>2</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="F102" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H102" s="3">
-        <v>1</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H103" s="3">
-        <v>1</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>